<commit_message>
Fix discrepancies in translation formatting
</commit_message>
<xml_diff>
--- a/i18n/fr.xlsx
+++ b/i18n/fr.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matej\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3953E686-2162-4186-80B4-FA97ED871142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" r:id="rId1"/>
@@ -15,21 +21,29 @@
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Birds!$A$1:$F$262</definedName>
     <definedName name="ExternalData_2" localSheetId="1" hidden="1">Bonuses!$A$1:$G$34</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Query - birds" description="Connection to the 'birds' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - birds" description="Connection to the 'birds' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=birds;Extended Properties=&quot;&quot;" command="SELECT * FROM [birds]"/>
   </connection>
-  <connection id="2" keepAlive="1" name="Query - bonuses" description="Connection to the 'bonuses' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Query - bonuses" description="Connection to the 'bonuses' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=bonuses;Extended Properties=&quot;&quot;" command="SELECT * FROM [bonuses]"/>
   </connection>
 </connections>
@@ -2552,15 +2566,9 @@
     <t>Oiseaux ayant des cartes glissées sous eux</t>
   </si>
   <si>
-    <t>Les termes incluent : aigrette, aile, bec, col, croupion, épaule, face, gorge, huppe, poitrine, queue, tête, ventre, yeux.</t>
-  </si>
-  <si>
     <t>Oiseaux valant moins de 4 points</t>
   </si>
   <si>
-    <t>Pour chaque colonne avec des oiseaux ayant 3 couleurs de pouvoirs différentes (marron, blanc, rose, bleu) :</t>
-  </si>
-  <si>
     <t>Oiseaux pouvant vivre dans plusieurs habitats</t>
   </si>
   <si>
@@ -2573,52 +2581,7 @@
     <t>Oiseaux avec 1 icône [seed]. Ils peuvent aussi avoir d'autres icônes.</t>
   </si>
   <si>
-    <t>ANATOMISTE</t>
-  </si>
-  <si>
-    <t>ORNITHOLOGUE DE BASSE-COUR</t>
-  </si>
-  <si>
-    <t>2-3 OISEAUX : 3[point]; 4+ OISEAUX : 7[point]</t>
-  </si>
-  <si>
-    <t>5-6 OISEAUX : 3[point]; 7+ OISEAUX : 6[point]</t>
-  </si>
-  <si>
-    <t>COMPORTEMENTALISTE</t>
-  </si>
-  <si>
     <t>Les oiseaux sans pouvoir comptent comme blanc.</t>
-  </si>
-  <si>
-    <t>3[point] PAR COLONNE</t>
-  </si>
-  <si>
-    <t>BAGUEUR D'OISEAUX</t>
-  </si>
-  <si>
-    <t>4-5 OISEAUX : 4[point]; 6+ OISEAUX : 7[point]</t>
-  </si>
-  <si>
-    <t>COMPTEUR D'OISEAUX</t>
-  </si>
-  <si>
-    <t>2[point] PAR OISEAU</t>
-  </si>
-  <si>
-    <t>MANGEOIRE</t>
-  </si>
-  <si>
-    <t>5-7 OISEAUX : 3[point]; 8+ OISEAUX : 7[point]</t>
-  </si>
-  <si>
-    <t>DIRECTEUR D'ÉLEVAGE</t>
-  </si>
-  <si>
-    <t>1[point] PAR OISEAU</t>
-  </si>
-  <si>
-    <t>CARTOGRAPHE</t>
   </si>
   <si>
     <t>Oiseaux avec des termes géographiques dans leur nom</t>
@@ -2648,189 +2611,81 @@
     </r>
   </si>
   <si>
-    <t>Ces termes incluent : Amérique, Baltimore, Californie, Canada, Caroline, Est, Inca, Islande, Mississippi, Ouest, Prairies, Prés, Rivage, Virginie.</t>
-  </si>
-  <si>
-    <t>SCIENTIFIQUE CITOYEN</t>
-  </si>
-  <si>
-    <t>4-6 OISEAUX : 3[point]; 7+ OISEAUX : 7[point]</t>
-  </si>
-  <si>
-    <t>DIÉTÉTICIEN</t>
-  </si>
-  <si>
     <t>Oiseaux coûtant 2 nourritures</t>
   </si>
   <si>
-    <t>2-3 OISEAUX : 3[point]; 4+ OISEAUX : 6[point]</t>
-  </si>
-  <si>
-    <t>ÉCOLOGISTE</t>
-  </si>
-  <si>
     <t>Oiseaux dans votre habitat le moins peuplé</t>
   </si>
   <si>
-    <t>Les égalités comptent : si vous avez 3 oiseaux dans chaque habitat, votre habitat le moins peuplé en compte 3.</t>
-  </si>
-  <si>
-    <t>CONSTRUCTEUR D'ENCLOS</t>
-  </si>
-  <si>
     <t>Oiseaux avec un nid [ground]</t>
   </si>
   <si>
     <t>Oiseaux ayant un nid de type [ground] ou [star]</t>
   </si>
   <si>
-    <t>ÉTHOLOGUE</t>
-  </si>
-  <si>
-    <t>Dans un de vos habitats :</t>
-  </si>
-  <si>
     <t>(marron, blanc, rose, bleu) Les oiseaux sans pouvoir comptent comme blanc.</t>
   </si>
   <si>
-    <t>2[point] PAR COULEUR DE POUVOIR</t>
-  </si>
-  <si>
-    <t>FAUCONNIER</t>
-  </si>
-  <si>
     <t>Oiseaux avec un pouvoir [predator]</t>
   </si>
   <si>
-    <t>GÉRANT DE PÊCHERIE</t>
-  </si>
-  <si>
     <t>Oiseaux qui mangent [fish]</t>
   </si>
   <si>
     <t>Oiseaux avec 1 icône [fish]. Ils peuvent aussi avoir d'autres icônes.</t>
   </si>
   <si>
-    <t>2-3 OISEAUX : 3[point]; 4+ OISEAUX : 8[point]</t>
-  </si>
-  <si>
-    <t>EXPERT EN CHAÎNE ALIMENTAIRE</t>
-  </si>
-  <si>
     <t>Oiseaux qui mangent [invertebrate] uniquement</t>
   </si>
   <si>
     <t>Oiseaux avec 1 icône [invertebrate] et aucune autre icône de nourriture.</t>
   </si>
   <si>
-    <t>FORESTIER</t>
-  </si>
-  <si>
     <t>Oiseaux vivant uniquement dans [forest]</t>
   </si>
   <si>
-    <t>3-4 OISEAUX : 4[point]; 5 OISEAUX : 8[point]</t>
-  </si>
-  <si>
-    <t>HISTORIEN</t>
-  </si>
-  <si>
     <t>Oiseaux portant le nom d'une personne</t>
   </si>
   <si>
     <t>Oiseaux portant le nom d'une personne. Ces noms sont soulignés sur les cartes Oiseau.</t>
   </si>
   <si>
-    <t>SPÉCIALISTE DES GRANDS OISEAUX</t>
-  </si>
-  <si>
     <t>Oiseaux avec une envergure de plus de 65 cm</t>
   </si>
   <si>
-    <t>4-5 OISEAUX : 3[point]; 6+ OISEAUX : 6[point]</t>
-  </si>
-  <si>
-    <t>CONSTRUCTEUR DE NICHOIR</t>
-  </si>
-  <si>
     <t>Oiseaux avec un nid [cavity]</t>
   </si>
   <si>
     <t>Oiseaux ayant un nid de type [cavity] ou [star]</t>
   </si>
   <si>
-    <t>EXPERT EN OMNIVORES</t>
-  </si>
-  <si>
-    <t>OOLOGISTE</t>
-  </si>
-  <si>
     <t>Oiseaux ayant au moins 1 œuf sur eux</t>
   </si>
   <si>
-    <t>7-8 OISEAUX : 3[point]; 9+ OISEAUX : 6[point]</t>
-  </si>
-  <si>
-    <t>SPÉCIALISTE DES PASSEREAUX</t>
-  </si>
-  <si>
     <t>Oiseaux avec une envergure de 30 cm ou moins</t>
   </si>
   <si>
-    <t>PHOTOGRAPHE</t>
-  </si>
-  <si>
     <t>Oiseaux avec une couleur dans leur nom</t>
   </si>
   <si>
-    <t>Les couleurs incluent : ardoisé, azuré, blanc, bleu, bronzé, brun, cendré, gris, indigo, jaune, neigeuse, noir, orangé, rose, rosée, rouge, rouilleux, roux/rousse, rubis, vert, violacé.</t>
-  </si>
-  <si>
-    <t>CONSTRUCTEUR DE PLATEFORME</t>
-  </si>
-  <si>
     <t>Oiseaux avec un nid [platform]</t>
   </si>
   <si>
     <t>Oiseaux ayant un nid de type [platform] ou [star]</t>
   </si>
   <si>
-    <t>GARDIEN DE PRAIRIE</t>
-  </si>
-  <si>
     <t>Oiseaux vivant uniquement dans [grassland]</t>
   </si>
   <si>
-    <t>EXPERT EN RONGEURS</t>
-  </si>
-  <si>
     <t>Oiseaux qui mangent [rodent]</t>
   </si>
   <si>
-    <t>PLANIFICATEUR</t>
-  </si>
-  <si>
     <t>Cartes Oiseau en main en fin de partie</t>
   </si>
   <si>
-    <t>5-7 OISEAUX : 4[point]; 8+ OISEAUX : 7[point]</t>
-  </si>
-  <si>
-    <t>VITICULTEUR</t>
-  </si>
-  <si>
     <t>Oiseaux qui mangent [fruit]</t>
   </si>
   <si>
-    <t>SCIENTIFIQUE EN ZONE HUMIDE</t>
-  </si>
-  <si>
-    <t>3-4 OISEAUX : 3[point]; 5 OISEAUX : 7[point]</t>
-  </si>
-  <si>
-    <t>JARDINIER ANIMALIER</t>
-  </si>
-  <si>
     <t>Oiseaux avec un nid [bowl]</t>
   </si>
   <si>
@@ -2850,12 +2705,6 @@
   </si>
   <si>
     <t>ACTIVATION</t>
-  </si>
-  <si>
-    <t>[automa] AUTO PERCHEUR</t>
-  </si>
-  <si>
-    <t>[automa] MEMBRE DE LA LPO</t>
   </si>
   <si>
     <t>Oiseaux qui valent 3 ou 4 points</t>
@@ -2895,11 +2744,176 @@
   <si>
     <t>Oiseaux avec 1 icône [fruit]. Ils peuvent aussi avoir d'autres icônes.</t>
   </si>
+  <si>
+    <t>Anatomiste</t>
+  </si>
+  <si>
+    <t>Ornithologue De Basse-Cour</t>
+  </si>
+  <si>
+    <t>Comportementaliste</t>
+  </si>
+  <si>
+    <t>Bagueur D'Oiseaux</t>
+  </si>
+  <si>
+    <t>Compteur D'Oiseaux</t>
+  </si>
+  <si>
+    <t>Mangeoire</t>
+  </si>
+  <si>
+    <t>Directeur D'Élevage</t>
+  </si>
+  <si>
+    <t>Cartographe</t>
+  </si>
+  <si>
+    <t>Scientifique Citoyen</t>
+  </si>
+  <si>
+    <t>Diététicien</t>
+  </si>
+  <si>
+    <t>Écologiste</t>
+  </si>
+  <si>
+    <t>Constructeur D'Enclos</t>
+  </si>
+  <si>
+    <t>Éthologue</t>
+  </si>
+  <si>
+    <t>Fauconnier</t>
+  </si>
+  <si>
+    <t>Gérant De Pêcherie</t>
+  </si>
+  <si>
+    <t>Expert En Chaîne Alimentaire</t>
+  </si>
+  <si>
+    <t>Forestier</t>
+  </si>
+  <si>
+    <t>Historien</t>
+  </si>
+  <si>
+    <t>Spécialiste Des Grands Oiseaux</t>
+  </si>
+  <si>
+    <t>Constructeur De Nichoir</t>
+  </si>
+  <si>
+    <t>Expert En Omnivores</t>
+  </si>
+  <si>
+    <t>Oologiste</t>
+  </si>
+  <si>
+    <t>Spécialiste Des Passereaux</t>
+  </si>
+  <si>
+    <t>Photographe</t>
+  </si>
+  <si>
+    <t>Constructeur De Plateforme</t>
+  </si>
+  <si>
+    <t>Gardien De Prairie</t>
+  </si>
+  <si>
+    <t>Expert En Rongeurs</t>
+  </si>
+  <si>
+    <t>Planificateur</t>
+  </si>
+  <si>
+    <t>Viticulteur</t>
+  </si>
+  <si>
+    <t>Scientifique En Zone Humide</t>
+  </si>
+  <si>
+    <t>Jardinier Animalier</t>
+  </si>
+  <si>
+    <t>3[point] par colonne</t>
+  </si>
+  <si>
+    <t>2[point] par oiseau</t>
+  </si>
+  <si>
+    <t>1[point] par oiseau</t>
+  </si>
+  <si>
+    <t>2[point] par couleur de pouvoir</t>
+  </si>
+  <si>
+    <t>[automa] Auto Percheur</t>
+  </si>
+  <si>
+    <t>[automa] Membre De La Lpo</t>
+  </si>
+  <si>
+    <t>Les termes incluent: aigrette, aile, bec, col, croupion, épaule, face, gorge, huppe, poitrine, queue, tête, ventre, yeux.</t>
+  </si>
+  <si>
+    <t>2-3 oiseaux: 3[point]; 4+ oiseaux: 7[point]</t>
+  </si>
+  <si>
+    <t>5-6 oiseaux: 3[point]; 7+ oiseaux: 6[point]</t>
+  </si>
+  <si>
+    <t>Pour chaque colonne avec des oiseaux ayant 3 couleurs de pouvoirs différentes (marron, blanc, rose, bleu):</t>
+  </si>
+  <si>
+    <t>4-5 oiseaux: 4[point]; 6+ oiseaux: 7[point]</t>
+  </si>
+  <si>
+    <t>5-7 oiseaux: 3[point]; 8+ oiseaux: 7[point]</t>
+  </si>
+  <si>
+    <t>Ces termes incluent: Amérique, Baltimore, Californie, Canada, Caroline, Est, Inca, Islande, Mississippi, Ouest, Prairies, Prés, Rivage, Virginie.</t>
+  </si>
+  <si>
+    <t>4-6 oiseaux: 3[point]; 7+ oiseaux: 7[point]</t>
+  </si>
+  <si>
+    <t>2-3 oiseaux: 3[point]; 4+ oiseaux: 6[point]</t>
+  </si>
+  <si>
+    <t>Les égalités comptent: si vous avez 3 oiseaux dans chaque habitat, votre habitat le moins peuplé en compte 3.</t>
+  </si>
+  <si>
+    <t>Dans un de vos habitats:</t>
+  </si>
+  <si>
+    <t>2-3 oiseaux: 3[point]; 4+ oiseaux: 8[point]</t>
+  </si>
+  <si>
+    <t>3-4 oiseaux: 4[point]; 5 oiseaux: 8[point]</t>
+  </si>
+  <si>
+    <t>4-5 oiseaux: 3[point]; 6+ oiseaux: 6[point]</t>
+  </si>
+  <si>
+    <t>7-8 oiseaux: 3[point]; 9+ oiseaux: 6[point]</t>
+  </si>
+  <si>
+    <t>Les couleurs incluent: ardoisé, azuré, blanc, bleu, bronzé, brun, cendré, gris, indigo, jaune, neigeuse, noir, orangé, rose, rosée, rouge, rouilleux, roux/rousse, rubis, vert, violacé.</t>
+  </si>
+  <si>
+    <t>5-7 oiseaux: 4[point]; 8+ oiseaux: 7[point]</t>
+  </si>
+  <si>
+    <t>3-4 oiseaux: 3[point]; 5 oiseaux: 7[point]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2972,9 +2986,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3027,7 +3039,9 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3047,7 +3061,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7">
     <queryTableFields count="6">
       <queryTableField id="1" name="id" tableColumnId="1"/>
@@ -3062,8 +3076,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="8">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_2" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh nextId="9">
     <queryTableFields count="7">
       <queryTableField id="1" name="id" tableColumnId="1"/>
       <queryTableField id="2" name="English name" tableColumnId="2"/>
@@ -3078,42 +3092,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="birds" displayName="birds" ref="A1:F262" tableType="queryTable" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:F262"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="birds" displayName="birds" ref="A1:F262" tableType="queryTable" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:F262" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="11"/>
-    <tableColumn id="2" uniqueName="2" name="English name" queryTableFieldId="2" dataDxfId="10"/>
-    <tableColumn id="3" uniqueName="3" name="Scientific name" queryTableFieldId="3" dataDxfId="9"/>
-    <tableColumn id="4" uniqueName="4" name="Common name" queryTableFieldId="4" dataDxfId="8"/>
-    <tableColumn id="5" uniqueName="5" name="Power text" queryTableFieldId="5" dataDxfId="7"/>
-    <tableColumn id="6" uniqueName="6" name="Note" queryTableFieldId="6" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="English name" queryTableFieldId="2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Scientific name" queryTableFieldId="3" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Common name" queryTableFieldId="4" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Power text" queryTableFieldId="5" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Note" queryTableFieldId="6" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="bonuses" displayName="bonuses" ref="A1:G34" tableType="queryTable" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:G34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="bonuses" displayName="bonuses" ref="A1:G34" tableType="queryTable" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:G34" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" uniqueName="2" name="English name" queryTableFieldId="2" dataDxfId="19"/>
-    <tableColumn id="3" uniqueName="3" name="Name" queryTableFieldId="3" dataDxfId="18"/>
-    <tableColumn id="4" uniqueName="4" name="Condition" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="5" uniqueName="5" name="Explanatory text" queryTableFieldId="5" dataDxfId="16"/>
-    <tableColumn id="6" uniqueName="6" name="VP" queryTableFieldId="6" dataDxfId="15"/>
-    <tableColumn id="7" uniqueName="7" name="Note" queryTableFieldId="7" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" uniqueName="1" name="id" queryTableFieldId="1" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" uniqueName="2" name="English name" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" uniqueName="3" name="Name" queryTableFieldId="3" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" uniqueName="4" name="Condition" queryTableFieldId="4" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" uniqueName="5" name="Explanatory text" queryTableFieldId="5" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" uniqueName="6" name="VP" queryTableFieldId="6" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" uniqueName="7" name="Note" queryTableFieldId="7" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:B6" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:B6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:B6" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="English name" dataDxfId="3"/>
-    <tableColumn id="2" name="Translated" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="English name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Translated" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3374,31 +3388,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F262"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.265625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3418,7 +3432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -3438,7 +3452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -3458,7 +3472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -3478,7 +3492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -3498,7 +3512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -3518,7 +3532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -3538,7 +3552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -3558,7 +3572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -3578,7 +3592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -3598,7 +3612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -3618,7 +3632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -3638,7 +3652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -3658,7 +3672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -3678,7 +3692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -3698,7 +3712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -3718,7 +3732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -3738,7 +3752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -3758,7 +3772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -3778,7 +3792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -3798,7 +3812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -3818,7 +3832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -3838,7 +3852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -3858,7 +3872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -3878,7 +3892,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -3898,7 +3912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -3918,7 +3932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -3938,7 +3952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -3958,7 +3972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -3978,7 +3992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -3998,7 +4012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -4018,7 +4032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -4038,7 +4052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -4058,7 +4072,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -4078,7 +4092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -4098,7 +4112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -4118,7 +4132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -4138,7 +4152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>38</v>
       </c>
@@ -4158,7 +4172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>39</v>
       </c>
@@ -4178,7 +4192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -4198,7 +4212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -4218,7 +4232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -4238,7 +4252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -4258,7 +4272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>44</v>
       </c>
@@ -4278,7 +4292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>45</v>
       </c>
@@ -4298,7 +4312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>46</v>
       </c>
@@ -4318,7 +4332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>47</v>
       </c>
@@ -4338,7 +4352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>48</v>
       </c>
@@ -4358,7 +4372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>49</v>
       </c>
@@ -4378,7 +4392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>50</v>
       </c>
@@ -4398,7 +4412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>51</v>
       </c>
@@ -4418,7 +4432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>52</v>
       </c>
@@ -4438,7 +4452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>53</v>
       </c>
@@ -4458,7 +4472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>54</v>
       </c>
@@ -4478,7 +4492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>55</v>
       </c>
@@ -4498,7 +4512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>56</v>
       </c>
@@ -4518,7 +4532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>57</v>
       </c>
@@ -4538,7 +4552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>58</v>
       </c>
@@ -4558,7 +4572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>59</v>
       </c>
@@ -4578,7 +4592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>60</v>
       </c>
@@ -4598,7 +4612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>61</v>
       </c>
@@ -4618,7 +4632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>62</v>
       </c>
@@ -4638,7 +4652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>63</v>
       </c>
@@ -4658,7 +4672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>64</v>
       </c>
@@ -4678,7 +4692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>65</v>
       </c>
@@ -4698,7 +4712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>66</v>
       </c>
@@ -4718,7 +4732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>67</v>
       </c>
@@ -4738,7 +4752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>68</v>
       </c>
@@ -4758,7 +4772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>69</v>
       </c>
@@ -4778,7 +4792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>70</v>
       </c>
@@ -4798,7 +4812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>71</v>
       </c>
@@ -4818,7 +4832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>72</v>
       </c>
@@ -4838,7 +4852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>73</v>
       </c>
@@ -4858,7 +4872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>74</v>
       </c>
@@ -4878,7 +4892,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>75</v>
       </c>
@@ -4898,7 +4912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>76</v>
       </c>
@@ -4918,7 +4932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>77</v>
       </c>
@@ -4938,7 +4952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>78</v>
       </c>
@@ -4958,7 +4972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>79</v>
       </c>
@@ -4978,7 +4992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>80</v>
       </c>
@@ -4998,7 +5012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>81</v>
       </c>
@@ -5018,7 +5032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>82</v>
       </c>
@@ -5038,7 +5052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>83</v>
       </c>
@@ -5058,7 +5072,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>84</v>
       </c>
@@ -5078,7 +5092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>85</v>
       </c>
@@ -5098,7 +5112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>86</v>
       </c>
@@ -5118,7 +5132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>87</v>
       </c>
@@ -5138,7 +5152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>88</v>
       </c>
@@ -5158,7 +5172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>89</v>
       </c>
@@ -5178,7 +5192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>90</v>
       </c>
@@ -5198,7 +5212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>91</v>
       </c>
@@ -5218,7 +5232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>92</v>
       </c>
@@ -5238,7 +5252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>93</v>
       </c>
@@ -5258,7 +5272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>94</v>
       </c>
@@ -5278,7 +5292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>95</v>
       </c>
@@ -5298,7 +5312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>96</v>
       </c>
@@ -5318,7 +5332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>97</v>
       </c>
@@ -5338,7 +5352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>98</v>
       </c>
@@ -5358,7 +5372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>99</v>
       </c>
@@ -5378,7 +5392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>100</v>
       </c>
@@ -5398,7 +5412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>101</v>
       </c>
@@ -5418,7 +5432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>102</v>
       </c>
@@ -5438,7 +5452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>103</v>
       </c>
@@ -5458,7 +5472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>104</v>
       </c>
@@ -5478,7 +5492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>105</v>
       </c>
@@ -5498,7 +5512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>106</v>
       </c>
@@ -5518,7 +5532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>107</v>
       </c>
@@ -5538,7 +5552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>108</v>
       </c>
@@ -5558,7 +5572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>109</v>
       </c>
@@ -5578,7 +5592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>110</v>
       </c>
@@ -5598,7 +5612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>111</v>
       </c>
@@ -5618,7 +5632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>112</v>
       </c>
@@ -5638,7 +5652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>113</v>
       </c>
@@ -5658,7 +5672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>114</v>
       </c>
@@ -5678,7 +5692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>115</v>
       </c>
@@ -5698,7 +5712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116" s="1">
         <v>116</v>
       </c>
@@ -5718,7 +5732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117" s="1">
         <v>117</v>
       </c>
@@ -5738,7 +5752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A118" s="1">
         <v>118</v>
       </c>
@@ -5758,7 +5772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119" s="1">
         <v>119</v>
       </c>
@@ -5778,7 +5792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A120" s="1">
         <v>120</v>
       </c>
@@ -5798,7 +5812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A121" s="1">
         <v>121</v>
       </c>
@@ -5818,7 +5832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A122" s="1">
         <v>122</v>
       </c>
@@ -5838,7 +5852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A123" s="1">
         <v>123</v>
       </c>
@@ -5858,7 +5872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A124" s="1">
         <v>124</v>
       </c>
@@ -5878,7 +5892,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A125" s="1">
         <v>125</v>
       </c>
@@ -5898,7 +5912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A126" s="1">
         <v>126</v>
       </c>
@@ -5918,7 +5932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A127" s="1">
         <v>127</v>
       </c>
@@ -5938,7 +5952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A128" s="1">
         <v>128</v>
       </c>
@@ -5958,7 +5972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A129" s="1">
         <v>129</v>
       </c>
@@ -5978,7 +5992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A130" s="1">
         <v>130</v>
       </c>
@@ -5998,7 +6012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A131" s="1">
         <v>131</v>
       </c>
@@ -6018,7 +6032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A132" s="1">
         <v>132</v>
       </c>
@@ -6038,7 +6052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A133" s="1">
         <v>133</v>
       </c>
@@ -6058,7 +6072,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A134" s="1">
         <v>134</v>
       </c>
@@ -6078,7 +6092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A135" s="1">
         <v>135</v>
       </c>
@@ -6098,7 +6112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A136" s="1">
         <v>136</v>
       </c>
@@ -6118,7 +6132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A137" s="1">
         <v>137</v>
       </c>
@@ -6138,7 +6152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A138" s="1">
         <v>138</v>
       </c>
@@ -6158,7 +6172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A139" s="1">
         <v>139</v>
       </c>
@@ -6178,7 +6192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A140" s="1">
         <v>140</v>
       </c>
@@ -6198,7 +6212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A141" s="1">
         <v>141</v>
       </c>
@@ -6218,7 +6232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A142" s="1">
         <v>142</v>
       </c>
@@ -6238,7 +6252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A143" s="1">
         <v>143</v>
       </c>
@@ -6258,7 +6272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A144" s="1">
         <v>144</v>
       </c>
@@ -6278,7 +6292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A145" s="1">
         <v>145</v>
       </c>
@@ -6298,7 +6312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A146" s="1">
         <v>146</v>
       </c>
@@ -6318,7 +6332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A147" s="1">
         <v>147</v>
       </c>
@@ -6338,7 +6352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A148" s="1">
         <v>148</v>
       </c>
@@ -6358,7 +6372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A149" s="1">
         <v>149</v>
       </c>
@@ -6378,7 +6392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A150" s="1">
         <v>150</v>
       </c>
@@ -6398,7 +6412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A151" s="1">
         <v>151</v>
       </c>
@@ -6418,7 +6432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A152" s="1">
         <v>152</v>
       </c>
@@ -6438,7 +6452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A153" s="1">
         <v>153</v>
       </c>
@@ -6458,7 +6472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A154" s="1">
         <v>154</v>
       </c>
@@ -6478,7 +6492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A155" s="1">
         <v>155</v>
       </c>
@@ -6498,7 +6512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A156" s="1">
         <v>156</v>
       </c>
@@ -6518,7 +6532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A157" s="1">
         <v>157</v>
       </c>
@@ -6538,7 +6552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A158" s="1">
         <v>158</v>
       </c>
@@ -6558,7 +6572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A159" s="1">
         <v>159</v>
       </c>
@@ -6578,7 +6592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A160" s="1">
         <v>160</v>
       </c>
@@ -6598,7 +6612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A161" s="1">
         <v>161</v>
       </c>
@@ -6618,7 +6632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A162" s="1">
         <v>162</v>
       </c>
@@ -6638,7 +6652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A163" s="1">
         <v>163</v>
       </c>
@@ -6658,7 +6672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A164" s="1">
         <v>164</v>
       </c>
@@ -6678,7 +6692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A165" s="1">
         <v>165</v>
       </c>
@@ -6698,7 +6712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A166" s="1">
         <v>166</v>
       </c>
@@ -6718,7 +6732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A167" s="1">
         <v>167</v>
       </c>
@@ -6738,7 +6752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A168" s="1">
         <v>168</v>
       </c>
@@ -6758,7 +6772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A169" s="1">
         <v>169</v>
       </c>
@@ -6778,7 +6792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A170" s="1">
         <v>170</v>
       </c>
@@ -6798,7 +6812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A171" s="1">
         <v>171</v>
       </c>
@@ -6818,7 +6832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A172" s="1">
         <v>172</v>
       </c>
@@ -6838,7 +6852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A173" s="1">
         <v>173</v>
       </c>
@@ -6858,7 +6872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A174" s="1">
         <v>174</v>
       </c>
@@ -6878,7 +6892,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A175" s="1">
         <v>175</v>
       </c>
@@ -6898,7 +6912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A176" s="1">
         <v>176</v>
       </c>
@@ -6918,7 +6932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A177" s="1">
         <v>177</v>
       </c>
@@ -6938,7 +6952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A178" s="1">
         <v>178</v>
       </c>
@@ -6958,7 +6972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A179" s="1">
         <v>179</v>
       </c>
@@ -6978,7 +6992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A180" s="1">
         <v>180</v>
       </c>
@@ -6998,7 +7012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="181" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A181" s="1">
         <v>181</v>
       </c>
@@ -7018,7 +7032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A182" s="1">
         <v>182</v>
       </c>
@@ -7038,7 +7052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A183" s="1">
         <v>183</v>
       </c>
@@ -7058,7 +7072,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A184" s="1">
         <v>184</v>
       </c>
@@ -7078,7 +7092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A185" s="1">
         <v>185</v>
       </c>
@@ -7098,7 +7112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A186" s="1">
         <v>186</v>
       </c>
@@ -7118,7 +7132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A187" s="1">
         <v>187</v>
       </c>
@@ -7138,7 +7152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A188" s="1">
         <v>188</v>
       </c>
@@ -7158,7 +7172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A189" s="1">
         <v>189</v>
       </c>
@@ -7178,7 +7192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A190" s="1">
         <v>190</v>
       </c>
@@ -7198,7 +7212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A191" s="1">
         <v>191</v>
       </c>
@@ -7218,7 +7232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A192" s="1">
         <v>192</v>
       </c>
@@ -7238,7 +7252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A193" s="1">
         <v>193</v>
       </c>
@@ -7258,7 +7272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A194" s="1">
         <v>194</v>
       </c>
@@ -7278,7 +7292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A195" s="1">
         <v>195</v>
       </c>
@@ -7298,7 +7312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A196" s="1">
         <v>196</v>
       </c>
@@ -7318,7 +7332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A197" s="1">
         <v>197</v>
       </c>
@@ -7338,7 +7352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A198" s="1">
         <v>198</v>
       </c>
@@ -7358,7 +7372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A199" s="1">
         <v>199</v>
       </c>
@@ -7378,7 +7392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="200" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A200" s="1">
         <v>200</v>
       </c>
@@ -7398,7 +7412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A201" s="1">
         <v>201</v>
       </c>
@@ -7418,7 +7432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A202" s="1">
         <v>203</v>
       </c>
@@ -7438,7 +7452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A203" s="1">
         <v>204</v>
       </c>
@@ -7458,7 +7472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A204" s="1">
         <v>205</v>
       </c>
@@ -7478,7 +7492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A205" s="1">
         <v>206</v>
       </c>
@@ -7498,7 +7512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A206" s="1">
         <v>207</v>
       </c>
@@ -7518,7 +7532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A207" s="1">
         <v>208</v>
       </c>
@@ -7538,7 +7552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A208" s="1">
         <v>209</v>
       </c>
@@ -7558,7 +7572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A209" s="1">
         <v>210</v>
       </c>
@@ -7578,7 +7592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A210" s="1">
         <v>211</v>
       </c>
@@ -7598,7 +7612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A211" s="1">
         <v>212</v>
       </c>
@@ -7618,7 +7632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A212" s="1">
         <v>213</v>
       </c>
@@ -7638,7 +7652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A213" s="1">
         <v>214</v>
       </c>
@@ -7658,7 +7672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A214" s="1">
         <v>215</v>
       </c>
@@ -7678,7 +7692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A215" s="1">
         <v>216</v>
       </c>
@@ -7698,7 +7712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A216" s="1">
         <v>217</v>
       </c>
@@ -7718,7 +7732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A217" s="1">
         <v>218</v>
       </c>
@@ -7738,7 +7752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="218" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A218" s="1">
         <v>219</v>
       </c>
@@ -7758,7 +7772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A219" s="1">
         <v>220</v>
       </c>
@@ -7778,7 +7792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A220" s="1">
         <v>221</v>
       </c>
@@ -7798,7 +7812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A221" s="1">
         <v>222</v>
       </c>
@@ -7818,7 +7832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="222" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A222" s="1">
         <v>223</v>
       </c>
@@ -7838,7 +7852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="223" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A223" s="1">
         <v>224</v>
       </c>
@@ -7858,7 +7872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A224" s="1">
         <v>225</v>
       </c>
@@ -7878,7 +7892,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A225" s="1">
         <v>226</v>
       </c>
@@ -7898,7 +7912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="226" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A226" s="1">
         <v>227</v>
       </c>
@@ -7918,7 +7932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="227" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A227" s="1">
         <v>228</v>
       </c>
@@ -7938,7 +7952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A228" s="1">
         <v>229</v>
       </c>
@@ -7958,7 +7972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="229" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A229" s="1">
         <v>230</v>
       </c>
@@ -7978,7 +7992,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="230" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A230" s="1">
         <v>231</v>
       </c>
@@ -7998,7 +8012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="231" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A231" s="1">
         <v>232</v>
       </c>
@@ -8018,7 +8032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A232" s="1">
         <v>233</v>
       </c>
@@ -8038,7 +8052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A233" s="1">
         <v>234</v>
       </c>
@@ -8058,7 +8072,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="234" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A234" s="1">
         <v>235</v>
       </c>
@@ -8078,7 +8092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="235" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A235" s="1">
         <v>236</v>
       </c>
@@ -8098,7 +8112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A236" s="1">
         <v>237</v>
       </c>
@@ -8118,7 +8132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A237" s="1">
         <v>238</v>
       </c>
@@ -8138,7 +8152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A238" s="1">
         <v>239</v>
       </c>
@@ -8158,7 +8172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="239" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A239" s="1">
         <v>240</v>
       </c>
@@ -8178,7 +8192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="240" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A240" s="1">
         <v>241</v>
       </c>
@@ -8198,7 +8212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="241" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A241" s="1">
         <v>242</v>
       </c>
@@ -8218,7 +8232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A242" s="1">
         <v>243</v>
       </c>
@@ -8238,7 +8252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="243" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A243" s="1">
         <v>244</v>
       </c>
@@ -8258,7 +8272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="244" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A244" s="1">
         <v>245</v>
       </c>
@@ -8278,7 +8292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="245" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A245" s="1">
         <v>246</v>
       </c>
@@ -8298,7 +8312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="246" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A246" s="1">
         <v>247</v>
       </c>
@@ -8318,7 +8332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="247" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A247" s="1">
         <v>248</v>
       </c>
@@ -8338,7 +8352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A248" s="1">
         <v>249</v>
       </c>
@@ -8358,7 +8372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="249" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A249" s="1">
         <v>250</v>
       </c>
@@ -8378,7 +8392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="250" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A250" s="1">
         <v>251</v>
       </c>
@@ -8398,7 +8412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A251" s="1">
         <v>252</v>
       </c>
@@ -8418,7 +8432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="252" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A252" s="1">
         <v>253</v>
       </c>
@@ -8438,7 +8452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="253" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A253" s="1">
         <v>254</v>
       </c>
@@ -8458,7 +8472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="254" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A254" s="1">
         <v>255</v>
       </c>
@@ -8478,7 +8492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A255" s="1">
         <v>256</v>
       </c>
@@ -8498,7 +8512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A256" s="1">
         <v>257</v>
       </c>
@@ -8518,7 +8532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A257" s="1">
         <v>258</v>
       </c>
@@ -8538,7 +8552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A258" s="1">
         <v>259</v>
       </c>
@@ -8558,7 +8572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A259" s="1">
         <v>260</v>
       </c>
@@ -8578,7 +8592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A260" s="1">
         <v>261</v>
       </c>
@@ -8598,7 +8612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A261" s="1">
         <v>262</v>
       </c>
@@ -8618,7 +8632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A262" s="1">
         <v>263</v>
       </c>
@@ -8647,26 +8661,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="106.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="44.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="106.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8689,7 +8703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -8697,22 +8711,22 @@
         <v>533</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>845</v>
+        <v>884</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>833</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>838</v>
+        <v>921</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>847</v>
+        <v>922</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1001</v>
       </c>
@@ -8720,22 +8734,22 @@
         <v>534</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>846</v>
+        <v>885</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>848</v>
+        <v>923</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>1002</v>
       </c>
@@ -8743,22 +8757,22 @@
         <v>535</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>849</v>
+        <v>886</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>840</v>
+        <v>924</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>851</v>
+        <v>915</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>1003</v>
       </c>
@@ -8766,22 +8780,22 @@
         <v>536</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>852</v>
+        <v>887</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>853</v>
+        <v>925</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>1004</v>
       </c>
@@ -8789,22 +8803,22 @@
         <v>537</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>854</v>
+        <v>888</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>855</v>
+        <v>916</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>1005</v>
       </c>
@@ -8812,22 +8826,22 @@
         <v>538</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>856</v>
+        <v>889</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>857</v>
+        <v>926</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>1006</v>
       </c>
@@ -8835,22 +8849,22 @@
         <v>539</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>858</v>
+        <v>890</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>862</v>
+        <v>845</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>859</v>
+        <v>917</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>1007</v>
       </c>
@@ -8858,22 +8872,22 @@
         <v>540</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>860</v>
+        <v>891</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>861</v>
+        <v>844</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>863</v>
+        <v>927</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>847</v>
+        <v>922</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>1008</v>
       </c>
@@ -8881,7 +8895,7 @@
         <v>541</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>864</v>
+        <v>892</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>837</v>
@@ -8890,13 +8904,13 @@
         <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>865</v>
+        <v>928</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>1009</v>
       </c>
@@ -8904,22 +8918,22 @@
         <v>542</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>866</v>
+        <v>893</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>867</v>
+        <v>846</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>868</v>
+        <v>929</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>1010</v>
       </c>
@@ -8927,22 +8941,22 @@
         <v>543</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>869</v>
+        <v>894</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>870</v>
+        <v>847</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>871</v>
+        <v>930</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>855</v>
+        <v>916</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>1011</v>
       </c>
@@ -8950,22 +8964,22 @@
         <v>544</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>872</v>
+        <v>895</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>873</v>
+        <v>848</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>874</v>
+        <v>849</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>853</v>
+        <v>925</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>1012</v>
       </c>
@@ -8973,22 +8987,22 @@
         <v>545</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>875</v>
+        <v>896</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>876</v>
+        <v>931</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>877</v>
+        <v>850</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>878</v>
+        <v>918</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>1013</v>
       </c>
@@ -8996,22 +9010,22 @@
         <v>546</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>879</v>
+        <v>897</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>880</v>
+        <v>851</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>855</v>
+        <v>916</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>1014</v>
       </c>
@@ -9019,22 +9033,22 @@
         <v>547</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>881</v>
+        <v>898</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>882</v>
+        <v>852</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>883</v>
+        <v>853</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>884</v>
+        <v>932</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>1015</v>
       </c>
@@ -9042,22 +9056,22 @@
         <v>548</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>885</v>
+        <v>899</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>886</v>
+        <v>854</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>887</v>
+        <v>855</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>855</v>
+        <v>916</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>1016</v>
       </c>
@@ -9065,22 +9079,22 @@
         <v>549</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>888</v>
+        <v>900</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>889</v>
+        <v>856</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>890</v>
+        <v>933</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>1017</v>
       </c>
@@ -9088,22 +9102,22 @@
         <v>550</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>891</v>
+        <v>901</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>892</v>
+        <v>857</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>893</v>
+        <v>858</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>855</v>
+        <v>916</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>1018</v>
       </c>
@@ -9111,22 +9125,22 @@
         <v>551</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>894</v>
+        <v>902</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>895</v>
+        <v>859</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>896</v>
+        <v>934</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>1019</v>
       </c>
@@ -9134,22 +9148,22 @@
         <v>552</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>898</v>
+        <v>860</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>899</v>
+        <v>861</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>853</v>
+        <v>925</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>1020</v>
       </c>
@@ -9157,7 +9171,7 @@
         <v>553</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>835</v>
@@ -9166,13 +9180,13 @@
         <v>836</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>855</v>
+        <v>916</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>1021</v>
       </c>
@@ -9180,22 +9194,22 @@
         <v>554</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>901</v>
+        <v>905</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>902</v>
+        <v>862</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>903</v>
+        <v>935</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>1022</v>
       </c>
@@ -9203,22 +9217,22 @@
         <v>555</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>905</v>
+        <v>863</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>896</v>
+        <v>934</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>1023</v>
       </c>
@@ -9226,22 +9240,22 @@
         <v>556</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>907</v>
+        <v>864</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>908</v>
+        <v>936</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>896</v>
+        <v>934</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>1024</v>
       </c>
@@ -9249,22 +9263,22 @@
         <v>557</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>910</v>
+        <v>865</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>911</v>
+        <v>866</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>853</v>
+        <v>925</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>1025</v>
       </c>
@@ -9272,22 +9286,22 @@
         <v>558</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>913</v>
+        <v>867</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>884</v>
+        <v>932</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>1026</v>
       </c>
@@ -9295,22 +9309,22 @@
         <v>559</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>915</v>
+        <v>868</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>937</v>
+        <v>882</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>855</v>
+        <v>916</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>1027</v>
       </c>
@@ -9318,22 +9332,22 @@
         <v>560</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>916</v>
+        <v>911</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>917</v>
+        <v>869</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>918</v>
+        <v>937</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>1028</v>
       </c>
@@ -9341,22 +9355,22 @@
         <v>561</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>919</v>
+        <v>912</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>920</v>
+        <v>870</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>938</v>
+        <v>883</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>847</v>
+        <v>922</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>1029</v>
       </c>
@@ -9364,19 +9378,19 @@
         <v>562</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>834</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>922</v>
+        <v>938</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>1030</v>
       </c>
@@ -9384,22 +9398,22 @@
         <v>563</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>923</v>
+        <v>914</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>924</v>
+        <v>871</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>925</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>853</v>
-      </c>
       <c r="G32" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>1031</v>
       </c>
@@ -9407,13 +9421,13 @@
         <v>564</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>931</v>
+        <v>919</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>933</v>
+        <v>878</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>935</v>
+        <v>880</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>8</v>
@@ -9422,7 +9436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>1032</v>
       </c>
@@ -9430,13 +9444,13 @@
         <v>565</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>932</v>
+        <v>920</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>934</v>
+        <v>879</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>936</v>
+        <v>881</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>8</v>
@@ -9455,21 +9469,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="21.59765625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -9477,44 +9491,44 @@
         <v>566</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>567</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>568</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>569</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>570</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>571</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>926</v>
+        <v>873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploy french language update
</commit_message>
<xml_diff>
--- a/i18n/fr.xlsx
+++ b/i18n/fr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Touniouk/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matej\Programming\wingsearch\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123F275D-4752-F449-B481-13CA17C406BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C963F6-9633-437E-A625-07E96FDB0C79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" r:id="rId1"/>
@@ -3806,9 +3806,6 @@
     <t>Défaussez 1 [egg] d’un de vos autres oiseaux pour gagner 2 [wild] de la réserve.</t>
   </si>
   <si>
-    <t>Choisissez 1 autre joueur. Pour chaque cube Action sur sa ligne [grasslandd], glissez 1 [card] de votre main sous cet oiseau, puis piochez autant de [card].</t>
-  </si>
-  <si>
     <t>Vous pouvez glisser des cartes à concurrence du nombre de cubes Action.</t>
   </si>
   <si>
@@ -3819,9 +3816,6 @@
   </si>
   <si>
     <t>Les nids [star] comptent comme des [bowl] ou [ground] pour cet oiseau.</t>
-  </si>
-  <si>
-    <t>Piochez 1 [cardd] face visible qui puisse être jouée dans [wetland].</t>
   </si>
   <si>
     <t>Choisissez 1 à 3 oiseaux dans votre [wetland]. Glissez 1 [card] de votre main sous chacun d’eux. Si vous le faites, piochez 1 [card].</t>
@@ -4480,9 +4474,6 @@
     <t>Faucon Brun</t>
   </si>
   <si>
-    <t>Regardez une [card] de la pioche. Si le coût en nourriture inclut [invertebrate] ou [mouse], glissez-la sous cet oiseau, sinon défaussez-la.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aigle d'Australie </t>
   </si>
   <si>
@@ -4499,9 +4490,6 @@
   </si>
   <si>
     <t>Élanion d'Australie</t>
-  </si>
-  <si>
-    <t>Relancez les dés de la mangeoire et gagnez 1 [rodednt], si disponible. Vous pouvez le donner à un autre joueur. Si vous le faites, pondez jusqu'à 3 [egg] sur cet oiseau.</t>
   </si>
   <si>
     <t xml:space="preserve">Pitohui Gris </t>
@@ -4693,6 +4681,18 @@
   </si>
   <si>
     <t>Vautour des palombes</t>
+  </si>
+  <si>
+    <t>Piochez 1 [card] face visible qui puisse être jouée dans [wetland].</t>
+  </si>
+  <si>
+    <t>Regardez une [card] de la pioche. Si le coût en nourriture inclut [invertebrate] ou [rodent], glissez-la sous cet oiseau, sinon défaussez-la.</t>
+  </si>
+  <si>
+    <t>Relancez les dés de la mangeoire et gagnez 1 [rodent], si disponible. Vous pouvez le donner à un autre joueur. Si vous le faites, pondez jusqu'à 3 [egg] sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Choisissez 1 autre joueur. Pour chaque cube Action sur sa ligne [grassland], glissez 1 [card] de votre main sous cet oiseau, puis piochez autant de [card].</t>
   </si>
 </sst>
 </file>
@@ -4824,7 +4824,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
     <dxf>
@@ -5279,22 +5279,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A285" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E286" sqref="E286"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="68" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E147" sqref="E147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="54.1640625" style="4" customWidth="1"/>
-    <col min="7" max="10" width="9.1640625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="54.109375" style="4" customWidth="1"/>
+    <col min="7" max="10" width="9.109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14" customHeight="1">
+    <row r="1" spans="1:10" ht="13.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5804,7 +5804,7 @@
         <v>590</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>8</v>
@@ -5982,10 +5982,10 @@
         <v>597</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14" t="s">
@@ -6034,7 +6034,7 @@
         <v>599</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>8</v>
@@ -6116,10 +6116,10 @@
         <v>602</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -6142,10 +6142,10 @@
         <v>603</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
@@ -6196,10 +6196,10 @@
         <v>605</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="14" t="s">
@@ -6276,7 +6276,7 @@
         <v>608</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>1224</v>
@@ -6300,7 +6300,7 @@
         <v>609</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>1214</v>
@@ -6432,7 +6432,7 @@
         <v>614</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>8</v>
@@ -6486,7 +6486,7 @@
         <v>616</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="F46" s="10" t="s">
         <v>8</v>
@@ -6664,7 +6664,7 @@
         <v>623</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="F53" s="12" t="s">
         <v>8</v>
@@ -6922,7 +6922,7 @@
         <v>633</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="F63" s="12" t="s">
         <v>1214</v>
@@ -6948,7 +6948,7 @@
         <v>634</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="F64" s="12" t="s">
         <v>8</v>
@@ -7026,7 +7026,7 @@
         <v>637</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="F67" s="12" t="s">
         <v>8</v>
@@ -7260,10 +7260,10 @@
         <v>646</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="G76" s="14"/>
       <c r="H76" s="14"/>
@@ -7286,10 +7286,10 @@
         <v>647</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="G77" s="14"/>
       <c r="H77" s="14"/>
@@ -7336,10 +7336,10 @@
         <v>649</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="F79" s="12" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="G79" s="14"/>
       <c r="H79" s="14"/>
@@ -7360,10 +7360,10 @@
         <v>650</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="G80" s="14"/>
       <c r="H80" s="14"/>
@@ -7384,10 +7384,10 @@
         <v>651</v>
       </c>
       <c r="E81" s="5" t="s">
+        <v>1236</v>
+      </c>
+      <c r="F81" s="5" t="s">
         <v>1237</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>1238</v>
       </c>
       <c r="G81" s="14"/>
       <c r="H81" s="14"/>
@@ -7410,10 +7410,10 @@
         <v>652</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="G82" s="14" t="s">
         <v>1133</v>
@@ -7562,10 +7562,10 @@
         <v>658</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="G88" s="14"/>
       <c r="H88" s="14"/>
@@ -7612,7 +7612,7 @@
         <v>660</v>
       </c>
       <c r="E90" s="10" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="F90" s="10" t="s">
         <v>8</v>
@@ -7734,7 +7734,7 @@
         <v>665</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>1178</v>
@@ -7760,7 +7760,7 @@
         <v>666</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>1185</v>
@@ -7786,7 +7786,7 @@
         <v>667</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>8</v>
@@ -7964,10 +7964,10 @@
         <v>674</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="G104" s="14"/>
       <c r="H104" s="14"/>
@@ -7988,7 +7988,7 @@
         <v>675</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="F105" s="5" t="s">
         <v>8</v>
@@ -8036,7 +8036,7 @@
         <v>677</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="F107" s="12" t="s">
         <v>8</v>
@@ -8088,10 +8088,10 @@
         <v>679</v>
       </c>
       <c r="E109" s="10" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="F109" s="10" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="G109" s="14"/>
       <c r="H109" s="14" t="s">
@@ -8117,7 +8117,7 @@
         <v>1198</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="G110" s="14"/>
       <c r="H110" s="14"/>
@@ -8188,7 +8188,7 @@
         <v>683</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="F113" s="5" t="s">
         <v>1221</v>
@@ -8236,10 +8236,10 @@
         <v>685</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="G115" s="14"/>
       <c r="H115" s="14"/>
@@ -8286,10 +8286,10 @@
         <v>687</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="F117" s="7" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="G117" s="14"/>
       <c r="H117" s="14"/>
@@ -8310,7 +8310,7 @@
         <v>688</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="F118" s="5" t="s">
         <v>1197</v>
@@ -8384,10 +8384,10 @@
         <v>691</v>
       </c>
       <c r="E121" s="12" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="F121" s="12" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="G121" s="14" t="s">
         <v>1133</v>
@@ -8412,10 +8412,10 @@
         <v>692</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="F122" s="7" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="G122" s="14"/>
       <c r="H122" s="14" t="s">
@@ -8438,7 +8438,7 @@
         <v>693</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="F123" s="5" t="s">
         <v>1185</v>
@@ -8540,10 +8540,10 @@
         <v>697</v>
       </c>
       <c r="E127" s="10" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="F127" s="10" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="G127" s="14"/>
       <c r="H127" s="14"/>
@@ -8566,10 +8566,10 @@
         <v>698</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="F128" s="11" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="G128" s="14"/>
       <c r="H128" s="14"/>
@@ -8638,10 +8638,10 @@
         <v>701</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="G131" s="14"/>
       <c r="H131" s="14"/>
@@ -8710,10 +8710,10 @@
         <v>704</v>
       </c>
       <c r="E134" s="12" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="F134" s="12" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="G134" s="14"/>
       <c r="H134" s="14"/>
@@ -8784,7 +8784,7 @@
         <v>707</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="F137" s="5" t="s">
         <v>8</v>
@@ -8808,10 +8808,10 @@
         <v>708</v>
       </c>
       <c r="E138" s="12" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="F138" s="12" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="G138" s="14"/>
       <c r="H138" s="14"/>
@@ -8884,7 +8884,7 @@
         <v>711</v>
       </c>
       <c r="E141" s="5" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="F141" s="5" t="s">
         <v>8</v>
@@ -8910,10 +8910,10 @@
         <v>712</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="G142" s="14"/>
       <c r="H142" s="14"/>
@@ -8939,7 +8939,7 @@
         <v>1198</v>
       </c>
       <c r="F143" s="12" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="G143" s="14"/>
       <c r="H143" s="14"/>
@@ -8962,7 +8962,7 @@
         <v>714</v>
       </c>
       <c r="E144" s="9" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="F144" s="9" t="s">
         <v>8</v>
@@ -8986,7 +8986,7 @@
         <v>715</v>
       </c>
       <c r="E145" s="10" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="F145" s="10" t="s">
         <v>1197</v>
@@ -9012,10 +9012,10 @@
         <v>716</v>
       </c>
       <c r="E146" s="12" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="F146" s="12" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="G146" s="14"/>
       <c r="H146" s="14"/>
@@ -9036,10 +9036,10 @@
         <v>717</v>
       </c>
       <c r="E147" s="12" t="s">
+        <v>1523</v>
+      </c>
+      <c r="F147" s="12" t="s">
         <v>1234</v>
-      </c>
-      <c r="F147" s="12" t="s">
-        <v>1235</v>
       </c>
       <c r="G147" s="14"/>
       <c r="H147" s="14"/>
@@ -9060,10 +9060,10 @@
         <v>718</v>
       </c>
       <c r="E148" s="5" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="F148" s="5" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="G148" s="14"/>
       <c r="H148" s="14"/>
@@ -9280,10 +9280,10 @@
         <v>727</v>
       </c>
       <c r="E157" s="9" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="F157" s="9" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="G157" s="14"/>
       <c r="H157" s="14"/>
@@ -9328,10 +9328,10 @@
         <v>729</v>
       </c>
       <c r="E159" s="7" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="F159" s="7" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="G159" s="14"/>
       <c r="H159" s="14"/>
@@ -9354,7 +9354,7 @@
         <v>730</v>
       </c>
       <c r="E160" s="10" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="F160" s="10" t="s">
         <v>8</v>
@@ -9404,7 +9404,7 @@
         <v>732</v>
       </c>
       <c r="E162" s="9" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="F162" s="9" t="s">
         <v>1185</v>
@@ -9478,10 +9478,10 @@
         <v>735</v>
       </c>
       <c r="E165" s="12" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="F165" s="12" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="G165" s="14" t="s">
         <v>1133</v>
@@ -9686,10 +9686,10 @@
         <v>743</v>
       </c>
       <c r="E173" s="5" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="F173" s="5" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="G173" s="14"/>
       <c r="H173" s="14"/>
@@ -9762,7 +9762,7 @@
         <v>746</v>
       </c>
       <c r="E176" s="5" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="F176" s="5" t="s">
         <v>8</v>
@@ -9786,7 +9786,7 @@
         <v>747</v>
       </c>
       <c r="E177" s="12" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="F177" s="12" t="s">
         <v>8</v>
@@ -9809,7 +9809,7 @@
         <v>360</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>1523</v>
+        <v>1519</v>
       </c>
       <c r="E178" s="9" t="s">
         <v>1176</v>
@@ -9860,10 +9860,10 @@
         <v>749</v>
       </c>
       <c r="E180" s="10" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="F180" s="10" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="G180" s="14"/>
       <c r="H180" s="14"/>
@@ -9956,7 +9956,7 @@
         <v>753</v>
       </c>
       <c r="E184" s="5" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="F184" s="5" t="s">
         <v>8</v>
@@ -10062,10 +10062,10 @@
         <v>757</v>
       </c>
       <c r="E188" s="5" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="F188" s="5" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="G188" s="14"/>
       <c r="H188" s="14"/>
@@ -10086,7 +10086,7 @@
         <v>758</v>
       </c>
       <c r="E189" s="10" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="F189" s="10" t="s">
         <v>8</v>
@@ -10188,7 +10188,7 @@
         <v>762</v>
       </c>
       <c r="E193" s="10" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="F193" s="10" t="s">
         <v>8</v>
@@ -10476,7 +10476,7 @@
         <v>773</v>
       </c>
       <c r="E204" s="5" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="F204" s="5" t="s">
         <v>8</v>
@@ -10820,10 +10820,10 @@
         <v>786</v>
       </c>
       <c r="E217" s="12" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="F217" s="12" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="G217" s="14"/>
       <c r="H217" s="14"/>
@@ -10894,7 +10894,7 @@
         <v>789</v>
       </c>
       <c r="E220" s="10" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="F220" s="10" t="s">
         <v>8</v>
@@ -10920,10 +10920,10 @@
         <v>790</v>
       </c>
       <c r="E221" s="12" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="F221" s="12" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="G221" s="14"/>
       <c r="H221" s="14"/>
@@ -10994,7 +10994,7 @@
         <v>793</v>
       </c>
       <c r="E224" s="5" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="F224" s="5" t="s">
         <v>1185</v>
@@ -11090,7 +11090,7 @@
         <v>797</v>
       </c>
       <c r="E228" s="5" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="F228" s="5" t="s">
         <v>8</v>
@@ -11140,7 +11140,7 @@
         <v>799</v>
       </c>
       <c r="E230" s="12" t="s">
-        <v>1239</v>
+        <v>1520</v>
       </c>
       <c r="F230" s="12" t="s">
         <v>1195</v>
@@ -11187,7 +11187,7 @@
         <v>468</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>1522</v>
+        <v>1518</v>
       </c>
       <c r="E232" s="7" t="s">
         <v>1179</v>
@@ -11314,10 +11314,10 @@
         <v>805</v>
       </c>
       <c r="E237" s="12" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="F237" s="12" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="G237" s="14" t="s">
         <v>1133</v>
@@ -11342,7 +11342,7 @@
         <v>806</v>
       </c>
       <c r="E238" s="12" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="F238" s="12" t="s">
         <v>8</v>
@@ -11394,10 +11394,10 @@
         <v>808</v>
       </c>
       <c r="E240" s="8" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="F240" s="8" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="G240" s="14"/>
       <c r="H240" s="14" t="s">
@@ -11636,7 +11636,7 @@
         <v>817</v>
       </c>
       <c r="E249" s="10" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="F249" s="10" t="s">
         <v>8</v>
@@ -11764,10 +11764,10 @@
         <v>822</v>
       </c>
       <c r="E254" s="10" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="F254" s="10" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="G254" s="14"/>
       <c r="H254" s="14"/>
@@ -11842,7 +11842,7 @@
         <v>825</v>
       </c>
       <c r="E257" s="10" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="F257" s="10" t="s">
         <v>8</v>
@@ -11997,13 +11997,13 @@
         <v>938</v>
       </c>
       <c r="D263" s="2" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="E263" s="5" t="s">
-        <v>1484</v>
+        <v>1480</v>
       </c>
       <c r="F263" s="5" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="G263" s="14"/>
       <c r="H263" s="14"/>
@@ -12023,10 +12023,10 @@
         <v>940</v>
       </c>
       <c r="D264" s="2" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="E264" s="5" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="F264" s="5"/>
       <c r="G264" s="14"/>
@@ -12047,10 +12047,10 @@
         <v>942</v>
       </c>
       <c r="D265" s="2" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="E265" s="12" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="F265" s="12"/>
       <c r="G265" s="14"/>
@@ -12071,13 +12071,13 @@
         <v>944</v>
       </c>
       <c r="D266" s="2" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="E266" s="12" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="F266" s="12" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="G266" s="14"/>
       <c r="H266" s="14" t="s">
@@ -12099,10 +12099,10 @@
         <v>946</v>
       </c>
       <c r="D267" s="2" t="s">
-        <v>1518</v>
+        <v>1514</v>
       </c>
       <c r="E267" s="5" t="s">
-        <v>1519</v>
+        <v>1515</v>
       </c>
       <c r="F267" s="5"/>
       <c r="G267" s="14"/>
@@ -12123,10 +12123,10 @@
         <v>948</v>
       </c>
       <c r="D268" s="2" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="E268" s="5" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="F268" s="5"/>
       <c r="G268" s="14"/>
@@ -12147,10 +12147,10 @@
         <v>950</v>
       </c>
       <c r="D269" s="2" t="s">
-        <v>1514</v>
+        <v>1510</v>
       </c>
       <c r="E269" s="5" t="s">
-        <v>1515</v>
+        <v>1511</v>
       </c>
       <c r="F269" s="5"/>
       <c r="G269" s="14"/>
@@ -12171,10 +12171,10 @@
         <v>952</v>
       </c>
       <c r="D270" s="2" t="s">
-        <v>1500</v>
+        <v>1496</v>
       </c>
       <c r="E270" s="12" t="s">
-        <v>1501</v>
+        <v>1497</v>
       </c>
       <c r="F270" s="12"/>
       <c r="G270" s="14"/>
@@ -12195,13 +12195,13 @@
         <v>954</v>
       </c>
       <c r="D271" s="2" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="E271" s="12" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="F271" s="12" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="G271" s="14"/>
       <c r="H271" s="14" t="s">
@@ -12221,10 +12221,10 @@
         <v>956</v>
       </c>
       <c r="D272" s="2" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="E272" s="5" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="F272" s="5"/>
       <c r="G272" s="14"/>
@@ -12245,13 +12245,13 @@
         <v>958</v>
       </c>
       <c r="D273" s="2" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E273" s="5" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F273" s="5" t="s">
         <v>1438</v>
-      </c>
-      <c r="E273" s="5" t="s">
-        <v>1439</v>
-      </c>
-      <c r="F273" s="5" t="s">
-        <v>1440</v>
       </c>
       <c r="G273" s="14"/>
       <c r="H273" s="14"/>
@@ -12271,13 +12271,13 @@
         <v>960</v>
       </c>
       <c r="D274" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="E274" s="12" t="s">
+        <v>1405</v>
+      </c>
+      <c r="F274" s="12" t="s">
         <v>1406</v>
-      </c>
-      <c r="E274" s="12" t="s">
-        <v>1407</v>
-      </c>
-      <c r="F274" s="12" t="s">
-        <v>1408</v>
       </c>
       <c r="G274" s="14"/>
       <c r="H274" s="14"/>
@@ -12297,13 +12297,13 @@
         <v>962</v>
       </c>
       <c r="D275" s="2" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
       <c r="E275" s="5" t="s">
-        <v>1460</v>
+        <v>1522</v>
       </c>
       <c r="F275" s="5" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="G275" s="14"/>
       <c r="H275" s="14" t="s">
@@ -12323,10 +12323,10 @@
         <v>964</v>
       </c>
       <c r="D276" s="2" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="E276" s="5" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="F276" s="5"/>
       <c r="G276" s="14"/>
@@ -12345,10 +12345,10 @@
         <v>966</v>
       </c>
       <c r="D277" s="2" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="E277" s="5" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="F277" s="5"/>
       <c r="G277" s="14"/>
@@ -12367,10 +12367,10 @@
         <v>968</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="E278" s="5" t="s">
-        <v>1453</v>
+        <v>1521</v>
       </c>
       <c r="F278" s="5"/>
       <c r="G278" s="14"/>
@@ -12391,13 +12391,13 @@
         <v>970</v>
       </c>
       <c r="D279" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="E279" s="10" t="s">
+        <v>1425</v>
+      </c>
+      <c r="F279" s="10" t="s">
         <v>1426</v>
-      </c>
-      <c r="E279" s="10" t="s">
-        <v>1427</v>
-      </c>
-      <c r="F279" s="10" t="s">
-        <v>1428</v>
       </c>
       <c r="G279" s="14"/>
       <c r="H279" s="14"/>
@@ -12415,13 +12415,13 @@
         <v>972</v>
       </c>
       <c r="D280" s="2" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E280" s="5" t="s">
         <v>1415</v>
       </c>
-      <c r="E280" s="5" t="s">
-        <v>1417</v>
-      </c>
       <c r="F280" s="5" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="G280" s="14"/>
       <c r="H280" s="14"/>
@@ -12439,10 +12439,10 @@
         <v>974</v>
       </c>
       <c r="D281" s="2" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="E281" s="5" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="F281" s="5"/>
       <c r="G281" s="14"/>
@@ -12463,10 +12463,10 @@
         <v>976</v>
       </c>
       <c r="D282" s="2" t="s">
-        <v>1516</v>
+        <v>1512</v>
       </c>
       <c r="E282" s="5" t="s">
-        <v>1517</v>
+        <v>1513</v>
       </c>
       <c r="F282" s="5"/>
       <c r="G282" s="14"/>
@@ -12485,10 +12485,10 @@
         <v>978</v>
       </c>
       <c r="D283" s="2" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="E283" s="12" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="F283" s="12"/>
       <c r="G283" s="14"/>
@@ -12509,10 +12509,10 @@
         <v>980</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="E284" s="5" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="F284" s="5"/>
       <c r="G284" s="14"/>
@@ -12531,10 +12531,10 @@
         <v>982</v>
       </c>
       <c r="D285" s="2" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="E285" s="5" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="F285" s="5"/>
       <c r="G285" s="14" t="s">
@@ -12557,13 +12557,13 @@
         <v>984</v>
       </c>
       <c r="D286" s="2" t="s">
+        <v>1343</v>
+      </c>
+      <c r="E286" s="12" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F286" s="12" t="s">
         <v>1345</v>
-      </c>
-      <c r="E286" s="12" t="s">
-        <v>1346</v>
-      </c>
-      <c r="F286" s="12" t="s">
-        <v>1347</v>
       </c>
       <c r="G286" s="14"/>
       <c r="H286" s="14" t="s">
@@ -12583,10 +12583,10 @@
         <v>986</v>
       </c>
       <c r="D287" s="2" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="E287" s="5" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="F287" s="5"/>
       <c r="G287" s="14"/>
@@ -12605,10 +12605,10 @@
         <v>988</v>
       </c>
       <c r="D288" s="2" t="s">
-        <v>1504</v>
+        <v>1500</v>
       </c>
       <c r="E288" s="8" t="s">
-        <v>1505</v>
+        <v>1501</v>
       </c>
       <c r="F288" s="8"/>
       <c r="G288" s="14" t="s">
@@ -12629,13 +12629,13 @@
         <v>990</v>
       </c>
       <c r="D289" s="2" t="s">
-        <v>1511</v>
+        <v>1507</v>
       </c>
       <c r="E289" s="5" t="s">
-        <v>1512</v>
+        <v>1508</v>
       </c>
       <c r="F289" s="5" t="s">
-        <v>1513</v>
+        <v>1509</v>
       </c>
       <c r="G289" s="14"/>
       <c r="H289" s="14"/>
@@ -12655,10 +12655,10 @@
         <v>992</v>
       </c>
       <c r="D290" s="2" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="E290" s="5" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="F290" s="5"/>
       <c r="G290" s="14"/>
@@ -12677,10 +12677,10 @@
         <v>994</v>
       </c>
       <c r="D291" s="2" t="s">
-        <v>1457</v>
+        <v>1454</v>
       </c>
       <c r="E291" s="12" t="s">
-        <v>1458</v>
+        <v>1455</v>
       </c>
       <c r="F291" s="12"/>
       <c r="G291" s="14"/>
@@ -12699,13 +12699,13 @@
         <v>996</v>
       </c>
       <c r="D292" s="2" t="s">
-        <v>1461</v>
+        <v>1457</v>
       </c>
       <c r="E292" s="5" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="F292" s="5" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="G292" s="14"/>
       <c r="H292" s="14"/>
@@ -12725,10 +12725,10 @@
         <v>998</v>
       </c>
       <c r="D293" s="2" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="E293" s="12" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="F293" s="12"/>
       <c r="G293" s="14"/>
@@ -12749,10 +12749,10 @@
         <v>1000</v>
       </c>
       <c r="D294" s="2" t="s">
-        <v>1503</v>
+        <v>1499</v>
       </c>
       <c r="E294" s="8" t="s">
-        <v>1502</v>
+        <v>1498</v>
       </c>
       <c r="F294" s="8"/>
       <c r="G294" s="14"/>
@@ -12773,13 +12773,13 @@
         <v>1002</v>
       </c>
       <c r="D295" s="2" t="s">
-        <v>1510</v>
+        <v>1506</v>
       </c>
       <c r="E295" s="5" t="s">
-        <v>1509</v>
+        <v>1505</v>
       </c>
       <c r="F295" s="5" t="s">
-        <v>1508</v>
+        <v>1504</v>
       </c>
       <c r="G295" s="14"/>
       <c r="H295" s="14"/>
@@ -12799,10 +12799,10 @@
         <v>1004</v>
       </c>
       <c r="D296" s="2" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="E296" s="12" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="F296" s="12"/>
       <c r="G296" s="14"/>
@@ -12823,10 +12823,10 @@
         <v>1006</v>
       </c>
       <c r="D297" s="2" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="E297" s="12" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="F297" s="12"/>
       <c r="G297" s="14"/>
@@ -12848,7 +12848,7 @@
         <v>1007</v>
       </c>
       <c r="E298" s="5" t="s">
-        <v>1489</v>
+        <v>1485</v>
       </c>
       <c r="F298" s="5"/>
       <c r="G298" s="14"/>
@@ -12867,13 +12867,13 @@
         <v>1010</v>
       </c>
       <c r="D299" s="2" t="s">
-        <v>1480</v>
+        <v>1476</v>
       </c>
       <c r="E299" s="5" t="s">
-        <v>1481</v>
+        <v>1477</v>
       </c>
       <c r="F299" s="5" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
       <c r="G299" s="14"/>
       <c r="H299" s="14" t="s">
@@ -12893,10 +12893,10 @@
         <v>1012</v>
       </c>
       <c r="D300" s="2" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="E300" s="5" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="F300" s="5"/>
       <c r="G300" s="14"/>
@@ -12917,10 +12917,10 @@
         <v>1014</v>
       </c>
       <c r="D301" s="2" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="E301" s="5" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="F301" s="5"/>
       <c r="G301" s="14"/>
@@ -12941,10 +12941,10 @@
         <v>1016</v>
       </c>
       <c r="D302" s="2" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="E302" s="5" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="F302" s="5"/>
       <c r="G302" s="14"/>
@@ -12963,13 +12963,13 @@
         <v>1018</v>
       </c>
       <c r="D303" s="2" t="s">
-        <v>1468</v>
+        <v>1464</v>
       </c>
       <c r="E303" s="5" t="s">
-        <v>1469</v>
+        <v>1465</v>
       </c>
       <c r="F303" s="5" t="s">
-        <v>1465</v>
+        <v>1461</v>
       </c>
       <c r="G303" s="14"/>
       <c r="H303" s="14"/>
@@ -12987,10 +12987,10 @@
         <v>1020</v>
       </c>
       <c r="D304" s="2" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="E304" s="12" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="F304" s="12"/>
       <c r="G304" s="14"/>
@@ -13009,10 +13009,10 @@
         <v>1022</v>
       </c>
       <c r="D305" s="2" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="E305" s="5" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="F305" s="5"/>
       <c r="G305" s="14"/>
@@ -13033,10 +13033,10 @@
         <v>1024</v>
       </c>
       <c r="D306" s="2" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="E306" s="12" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="F306" s="12"/>
       <c r="G306" s="14"/>
@@ -13055,13 +13055,13 @@
         <v>1026</v>
       </c>
       <c r="D307" s="2" t="s">
+        <v>1395</v>
+      </c>
+      <c r="E307" s="12" t="s">
+        <v>1396</v>
+      </c>
+      <c r="F307" s="12" t="s">
         <v>1397</v>
-      </c>
-      <c r="E307" s="12" t="s">
-        <v>1398</v>
-      </c>
-      <c r="F307" s="12" t="s">
-        <v>1399</v>
       </c>
       <c r="G307" s="14"/>
       <c r="H307" s="14"/>
@@ -13079,13 +13079,13 @@
         <v>1028</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>1506</v>
+        <v>1502</v>
       </c>
       <c r="E308" s="5" t="s">
-        <v>1507</v>
+        <v>1503</v>
       </c>
       <c r="F308" s="5" t="s">
-        <v>1508</v>
+        <v>1504</v>
       </c>
       <c r="G308" s="14"/>
       <c r="H308" s="14"/>
@@ -13103,10 +13103,10 @@
         <v>1030</v>
       </c>
       <c r="D309" s="2" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="E309" s="7" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="F309" s="7"/>
       <c r="G309" s="14"/>
@@ -13127,13 +13127,13 @@
         <v>1032</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="E310" s="12" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="F310" s="12" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="G310" s="14"/>
       <c r="H310" s="14"/>
@@ -13151,13 +13151,13 @@
         <v>1034</v>
       </c>
       <c r="D311" s="2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="E311" s="5" t="s">
+        <v>1428</v>
+      </c>
+      <c r="F311" s="5" t="s">
         <v>1429</v>
-      </c>
-      <c r="E311" s="5" t="s">
-        <v>1430</v>
-      </c>
-      <c r="F311" s="5" t="s">
-        <v>1431</v>
       </c>
       <c r="G311" s="14" t="s">
         <v>1133</v>
@@ -13177,10 +13177,10 @@
         <v>1036</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="E312" s="12" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="F312" s="12"/>
       <c r="G312" s="14"/>
@@ -13199,13 +13199,13 @@
         <v>1038</v>
       </c>
       <c r="D313" s="2" t="s">
+        <v>1350</v>
+      </c>
+      <c r="E313" s="5" t="s">
+        <v>1351</v>
+      </c>
+      <c r="F313" s="5" t="s">
         <v>1352</v>
-      </c>
-      <c r="E313" s="5" t="s">
-        <v>1353</v>
-      </c>
-      <c r="F313" s="5" t="s">
-        <v>1354</v>
       </c>
       <c r="G313" s="14"/>
       <c r="H313" s="14"/>
@@ -13223,10 +13223,10 @@
         <v>1040</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="E314" s="5" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="F314" s="5"/>
       <c r="G314" s="14"/>
@@ -13245,13 +13245,13 @@
         <v>1042</v>
       </c>
       <c r="D315" s="2" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="E315" s="7" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="F315" s="7" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="G315" s="14" t="s">
         <v>1133</v>
@@ -13271,13 +13271,13 @@
         <v>1044</v>
       </c>
       <c r="D316" s="2" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E316" s="5" t="s">
         <v>1334</v>
       </c>
-      <c r="E316" s="5" t="s">
-        <v>1336</v>
-      </c>
       <c r="F316" s="5" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="G316" s="14"/>
       <c r="H316" s="14" t="s">
@@ -13297,10 +13297,10 @@
         <v>1046</v>
       </c>
       <c r="D317" s="2" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="E317" s="5" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="F317" s="5"/>
       <c r="G317" s="14"/>
@@ -13319,10 +13319,10 @@
         <v>1048</v>
       </c>
       <c r="D318" s="2" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="E318" s="5" t="s">
-        <v>1477</v>
+        <v>1473</v>
       </c>
       <c r="F318" s="5"/>
       <c r="G318" s="14"/>
@@ -13343,13 +13343,13 @@
         <v>1050</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="E319" s="7" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="F319" s="7" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="G319" s="14"/>
       <c r="H319" s="14"/>
@@ -13369,13 +13369,13 @@
         <v>1052</v>
       </c>
       <c r="D320" s="2" t="s">
+        <v>1389</v>
+      </c>
+      <c r="E320" s="5" t="s">
+        <v>1390</v>
+      </c>
+      <c r="F320" s="5" t="s">
         <v>1391</v>
-      </c>
-      <c r="E320" s="5" t="s">
-        <v>1392</v>
-      </c>
-      <c r="F320" s="5" t="s">
-        <v>1393</v>
       </c>
       <c r="G320" s="14" t="s">
         <v>1133</v>
@@ -13395,10 +13395,10 @@
         <v>1054</v>
       </c>
       <c r="D321" s="2" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="E321" s="12" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="F321" s="12"/>
       <c r="G321" s="14"/>
@@ -13417,10 +13417,10 @@
         <v>1056</v>
       </c>
       <c r="D322" s="2" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="E322" s="5" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="F322" s="5"/>
       <c r="G322" s="14"/>
@@ -13441,10 +13441,10 @@
         <v>1058</v>
       </c>
       <c r="D323" s="2" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="E323" s="12" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="F323" s="12"/>
       <c r="G323" s="14"/>
@@ -13463,10 +13463,10 @@
         <v>1060</v>
       </c>
       <c r="D324" s="2" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="E324" s="5" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="F324" s="5"/>
       <c r="G324" s="14" t="s">
@@ -13489,10 +13489,10 @@
         <v>1062</v>
       </c>
       <c r="D325" s="2" t="s">
-        <v>1478</v>
+        <v>1474</v>
       </c>
       <c r="E325" s="12" t="s">
-        <v>1479</v>
+        <v>1475</v>
       </c>
       <c r="F325" s="12"/>
       <c r="G325" s="14"/>
@@ -13511,10 +13511,10 @@
         <v>1064</v>
       </c>
       <c r="D326" s="2" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="E326" s="5" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="F326" s="5"/>
       <c r="G326" s="14"/>
@@ -13535,13 +13535,13 @@
         <v>1066</v>
       </c>
       <c r="D327" s="2" t="s">
+        <v>1384</v>
+      </c>
+      <c r="E327" s="12" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F327" s="12" t="s">
         <v>1386</v>
-      </c>
-      <c r="E327" s="12" t="s">
-        <v>1387</v>
-      </c>
-      <c r="F327" s="12" t="s">
-        <v>1388</v>
       </c>
       <c r="G327" s="14"/>
       <c r="H327" s="14"/>
@@ -13559,10 +13559,10 @@
         <v>1068</v>
       </c>
       <c r="D328" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="E328" s="12" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="F328" s="12"/>
       <c r="G328" s="14"/>
@@ -13583,10 +13583,10 @@
         <v>1070</v>
       </c>
       <c r="D329" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="E329" s="12" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="F329" s="12"/>
       <c r="G329" s="14" t="s">
@@ -13609,13 +13609,13 @@
         <v>1072</v>
       </c>
       <c r="D330" s="2" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E330" s="5" t="s">
         <v>1403</v>
       </c>
-      <c r="E330" s="5" t="s">
-        <v>1405</v>
-      </c>
       <c r="F330" s="5" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="G330" s="14" t="s">
         <v>1133</v>
@@ -13637,10 +13637,10 @@
         <v>1074</v>
       </c>
       <c r="D331" s="2" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="E331" s="12" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="F331" s="12"/>
       <c r="G331" s="14" t="s">
@@ -13663,10 +13663,10 @@
         <v>1076</v>
       </c>
       <c r="D332" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="E332" s="12" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="F332" s="12"/>
       <c r="G332" s="14"/>
@@ -13687,10 +13687,10 @@
         <v>1078</v>
       </c>
       <c r="D333" s="2" t="s">
-        <v>1495</v>
+        <v>1491</v>
       </c>
       <c r="E333" s="12" t="s">
-        <v>1496</v>
+        <v>1492</v>
       </c>
       <c r="F333" s="12"/>
       <c r="G333" s="14"/>
@@ -13709,10 +13709,10 @@
         <v>1080</v>
       </c>
       <c r="D334" s="2" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="E334" s="5" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="F334" s="5"/>
       <c r="G334" s="14"/>
@@ -13733,13 +13733,13 @@
         <v>1082</v>
       </c>
       <c r="D335" s="2" t="s">
+        <v>1364</v>
+      </c>
+      <c r="E335" s="5" t="s">
+        <v>1365</v>
+      </c>
+      <c r="F335" s="5" t="s">
         <v>1366</v>
-      </c>
-      <c r="E335" s="5" t="s">
-        <v>1367</v>
-      </c>
-      <c r="F335" s="5" t="s">
-        <v>1368</v>
       </c>
       <c r="G335" s="14"/>
       <c r="H335" s="14"/>
@@ -13757,10 +13757,10 @@
         <v>1084</v>
       </c>
       <c r="D336" s="2" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="E336" s="5" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="F336" s="5"/>
       <c r="G336" s="14"/>
@@ -13781,10 +13781,10 @@
         <v>1086</v>
       </c>
       <c r="D337" s="2" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="E337" s="5" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="F337" s="5"/>
       <c r="G337" s="14"/>
@@ -13805,10 +13805,10 @@
         <v>1088</v>
       </c>
       <c r="D338" s="2" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="E338" s="5" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="F338" s="5"/>
       <c r="G338" s="14" t="s">
@@ -13831,13 +13831,13 @@
         <v>1090</v>
       </c>
       <c r="D339" s="2" t="s">
-        <v>1473</v>
+        <v>1469</v>
       </c>
       <c r="E339" s="12" t="s">
-        <v>1474</v>
+        <v>1470</v>
       </c>
       <c r="F339" s="12" t="s">
-        <v>1475</v>
+        <v>1471</v>
       </c>
       <c r="G339" s="14"/>
       <c r="H339" s="14"/>
@@ -13855,10 +13855,10 @@
         <v>1092</v>
       </c>
       <c r="D340" s="2" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="E340" s="5" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="F340" s="5"/>
       <c r="G340" s="14" t="s">
@@ -13881,10 +13881,10 @@
         <v>1094</v>
       </c>
       <c r="D341" s="2" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
       <c r="E341" s="5" t="s">
-        <v>1521</v>
+        <v>1517</v>
       </c>
       <c r="F341" s="5"/>
       <c r="G341" s="14"/>
@@ -13903,13 +13903,13 @@
         <v>1096</v>
       </c>
       <c r="D342" s="2" t="s">
-        <v>1497</v>
+        <v>1493</v>
       </c>
       <c r="E342" s="5" t="s">
-        <v>1498</v>
+        <v>1494</v>
       </c>
       <c r="F342" s="5" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
       <c r="G342" s="14"/>
       <c r="H342" s="14"/>
@@ -13927,10 +13927,10 @@
         <v>1098</v>
       </c>
       <c r="D343" s="2" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="E343" s="12" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="F343" s="12"/>
       <c r="G343" s="14"/>
@@ -13951,13 +13951,13 @@
         <v>1100</v>
       </c>
       <c r="D344" s="2" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="E344" s="8" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="F344" s="8" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="G344" s="14"/>
       <c r="H344" s="14"/>
@@ -13975,13 +13975,13 @@
         <v>1102</v>
       </c>
       <c r="D345" s="2" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E345" s="5" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F345" s="5" t="s">
         <v>1394</v>
-      </c>
-      <c r="E345" s="5" t="s">
-        <v>1395</v>
-      </c>
-      <c r="F345" s="5" t="s">
-        <v>1396</v>
       </c>
       <c r="G345" s="14"/>
       <c r="H345" s="14"/>
@@ -13999,10 +13999,10 @@
         <v>1104</v>
       </c>
       <c r="D346" s="2" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="E346" s="5" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="F346" s="5"/>
       <c r="G346" s="14"/>
@@ -14021,10 +14021,10 @@
         <v>1106</v>
       </c>
       <c r="D347" s="2" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="E347" s="12" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="F347" s="12"/>
       <c r="G347" s="14" t="s">
@@ -14047,13 +14047,13 @@
         <v>1108</v>
       </c>
       <c r="D348" s="2" t="s">
-        <v>1490</v>
+        <v>1486</v>
       </c>
       <c r="E348" s="12" t="s">
-        <v>1491</v>
+        <v>1487</v>
       </c>
       <c r="F348" s="12" t="s">
-        <v>1492</v>
+        <v>1488</v>
       </c>
       <c r="G348" s="14"/>
       <c r="H348" s="14"/>
@@ -14071,13 +14071,13 @@
         <v>1110</v>
       </c>
       <c r="D349" s="2" t="s">
-        <v>1463</v>
+        <v>1459</v>
       </c>
       <c r="E349" s="5" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="F349" s="5" t="s">
-        <v>1465</v>
+        <v>1461</v>
       </c>
       <c r="G349" s="14"/>
       <c r="H349" s="14"/>
@@ -14097,13 +14097,13 @@
         <v>1112</v>
       </c>
       <c r="D350" s="2" t="s">
-        <v>1494</v>
+        <v>1490</v>
       </c>
       <c r="E350" s="8" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
       <c r="F350" s="8" t="s">
-        <v>1492</v>
+        <v>1488</v>
       </c>
       <c r="G350" s="14"/>
       <c r="H350" s="14"/>
@@ -14121,13 +14121,13 @@
         <v>1114</v>
       </c>
       <c r="D351" s="2" t="s">
-        <v>1454</v>
+        <v>1451</v>
       </c>
       <c r="E351" s="12" t="s">
-        <v>1455</v>
+        <v>1452</v>
       </c>
       <c r="F351" s="12" t="s">
-        <v>1456</v>
+        <v>1453</v>
       </c>
       <c r="G351" s="14"/>
       <c r="H351" s="14" t="s">
@@ -14147,10 +14147,10 @@
         <v>1116</v>
       </c>
       <c r="D352" s="2" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="E352" s="5" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="F352" s="5"/>
       <c r="G352" s="14"/>
@@ -14169,13 +14169,13 @@
         <v>1118</v>
       </c>
       <c r="D353" s="2" t="s">
-        <v>1466</v>
+        <v>1462</v>
       </c>
       <c r="E353" s="5" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
       <c r="F353" s="5" t="s">
-        <v>1465</v>
+        <v>1461</v>
       </c>
       <c r="G353" s="14" t="s">
         <v>1133</v>
@@ -14197,10 +14197,10 @@
         <v>1120</v>
       </c>
       <c r="D354" s="2" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="E354" s="5" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="F354" s="5"/>
       <c r="G354" s="14" t="s">
@@ -14223,13 +14223,13 @@
         <v>1122</v>
       </c>
       <c r="D355" s="2" t="s">
-        <v>1470</v>
+        <v>1466</v>
       </c>
       <c r="E355" s="5" t="s">
-        <v>1471</v>
+        <v>1467</v>
       </c>
       <c r="F355" s="5" t="s">
-        <v>1472</v>
+        <v>1468</v>
       </c>
       <c r="G355" s="14" t="s">
         <v>1133</v>
@@ -14251,13 +14251,13 @@
         <v>1124</v>
       </c>
       <c r="D356" s="2" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="E356" s="7" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="F356" s="7" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="G356" s="14"/>
       <c r="H356" s="14"/>
@@ -14275,13 +14275,13 @@
         <v>1126</v>
       </c>
       <c r="D357" s="2" t="s">
-        <v>1486</v>
+        <v>1482</v>
       </c>
       <c r="E357" s="5" t="s">
-        <v>1487</v>
+        <v>1483</v>
       </c>
       <c r="F357" s="5" t="s">
-        <v>1488</v>
+        <v>1484</v>
       </c>
       <c r="G357" s="14" t="s">
         <v>1133</v>
@@ -14306,16 +14306,16 @@
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="106.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="44.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="106.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
@@ -15179,11 +15179,11 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="21.44140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
@@ -15226,7 +15226,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="6" spans="1:2" customFormat="1">
+    <row r="6" spans="1:2" customFormat="1" ht="14.4">
       <c r="A6" t="s">
         <v>1132</v>
       </c>

</xml_diff>

<commit_message>
Add French translations to the Asia expansion
</commit_message>
<xml_diff>
--- a/i18n/fr.xlsx
+++ b/i18n/fr.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\wingsearch\i18n\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pary754\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850BE34A-F068-492B-A3A1-0E91E18D9EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D01F6A-D8C0-4D64-A25D-8BE05180D254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="ExternalData_1" localSheetId="0">Birds!$A$1:$G$357</definedName>
     <definedName name="ExternalData_2" localSheetId="1">Bonuses!$A$1:$H$39</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2956" uniqueCount="1827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3265" uniqueCount="2055">
   <si>
     <t>id</t>
   </si>
@@ -5650,6 +5650,745 @@
   <si>
     <t>Autour des palombes</t>
   </si>
+  <si>
+    <t>Pondez 2 [egg] sur chaque autre oiseau dans cette colonne.</t>
+  </si>
+  <si>
+    <t>Quand un autre joueur effectue l'action "Pondre des œufs", cet oiseau pond 1 [egg] sur un autre oiseau avec un nid [platform]. En utilisant ce pouvoir, vous pouvez pondre 3 œufs de plus que la limite habituelle.</t>
+  </si>
+  <si>
+    <t>Dépasser la limite d'œufs : lorsque vous activez cet oiseau, vous pouvez utiliser le pouvoir pour pondre un œuf sur un oiseau qui a déjà atteint sa limite d'œufs, comme indiqué dans la description du pouvoir. Ce pouvoir n'affecte aucune autre action du jeu, la limite d'œufs continue à s'appliquer par la suite. Un oiseau qui possède plus d'œufs que sa limite d'œufs compte pour la carte Bonus Thériogénologue Aviaire. Cette carte ne permet pas aux oiseaux qui n'ont pas de symbole de Nid, et donc pas de limite d'œufs, de recevoir des œufs.</t>
+  </si>
+  <si>
+    <t>Gagnez 1 [invertebrate], [seed], ou [fruit] de la réserve.</t>
+  </si>
+  <si>
+    <t>Glissez jusqu'à 3 [card] de votre main sous cet oiseau. Si vous glissez au moins 1 [card], pondez 1 [egg] sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Pondez 1 [egg] sur chaque oiseau adjacent à celui-ci (à droite et à gauche uniquement).</t>
+  </si>
+  <si>
+    <t>Colombine turvert</t>
+  </si>
+  <si>
+    <t>Coucou koël</t>
+  </si>
+  <si>
+    <t>Mésange azurée</t>
+  </si>
+  <si>
+    <t>Tisserin baya</t>
+  </si>
+  <si>
+    <t>Panure à moustaches</t>
+  </si>
+  <si>
+    <t>Cigogne noire</t>
+  </si>
+  <si>
+    <t>Pondez 1 [egg] sur cet oiseau pour chaque autre oiseau dans sa colonne avec au moins 1 œuf.</t>
+  </si>
+  <si>
+    <t>Drongo royal noir</t>
+  </si>
+  <si>
+    <t>Defaussez autant de [card] du plateau que vous les souhaitez, puis remplissez-le à nouveau. Si au moins un des oiseaux défaussés est un oiseau de [grassland], pondez 1 [egg] sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>L'oiseau défaussé peut posséder plusieurs symboles d'habitat, mais il doit avoir un symbole de prairie afin de compter pour ce pouvoir.</t>
+  </si>
+  <si>
+    <t>Loriot noir de Chine</t>
+  </si>
+  <si>
+    <t>Si vous avec utilisé les 4 actions lors de cette manche, gagnez 1 [wild] de la réserve, pondez 1 [egg] sur un oiseau de votre choix, et piochez 1 [card].</t>
+  </si>
+  <si>
+    <t>A la fin de la manche, si vous avez des cubes Action sur les 4 zones de gauche de votre plateau Joueur, vous pouvez effectuer les 3 actions indiquées sur cette carte. Effectuez les actions dans l'ordre.</t>
+  </si>
+  <si>
+    <t>Monticole merle-bleu</t>
+  </si>
+  <si>
+    <t>Si cet oiseau n'a pas d'oiseaux à sa droite, vous pouvez le déplacer (seulement la carte) sur le plateau du joueur à votre gauche (vous choisissez son habitat). Si vous le faites, piochez 3 [card].</t>
+  </si>
+  <si>
+    <t>Lorsque vous déplacez cet oiseau sur le plateau d'un autre joueur, placez-le sur l'emplacement vide le plusà gauche de n'importe quel habitat. S'il n'y a aucun emplacement de libre dans un habitat, vous ne pouvez pas y déplacer l'oiseau. Défaussez les oeufs sur cette carte, les jetons qui y sont stockés et les cartes qui ont été glissées dessous. Le joueur à qui vous donnez cet oiseau ne peut pas le refuser.</t>
+  </si>
+  <si>
+    <t>Milan à tête blanche</t>
+  </si>
+  <si>
+    <t>Choisissez 3 [die]. Lancez-les jusqu'à 3 fois. A chaque fois, si vous obtenez au moins 1 [fish] ou [rodent], stockez en 1 ici. Sinon, arrêtez de lancer les dés et défaussez toute la nourriture stockée sur l'oiseau lors de ce tour.</t>
+  </si>
+  <si>
+    <t>Ces pouvoirs sont des paris risqués. Après chaque lancer de dé(s), vérifiez si vous avez réussi ou échoué. Lorsque vous échouez, vous ne pouvez plus recommencer, le pouvoir a fini de s activer. Vous pouvez aussi choisir de vous arrêter et de ne pas relancer les dés à tout moment. Cela vous permet d'éviter d'échouer et de perdre ce que vous auriez gagné.
+Si vous échouez, vous devez vous encier et défausser toute la nourriture stockée sur cet oiseau lors de cette activation du pouvoir.
+Si vous réussissez, stockez l nourriture de la reserve sur cet oiseau (ne stockez pas plus d'un jeton après chaque lancer). Si vous avez lancé les dés moins de 3 fois au cours de cette activation du pouvoir, décidez si vous souhaitez les relancer.</t>
+  </si>
+  <si>
+    <t>Pinson du nord</t>
+  </si>
+  <si>
+    <t>Piochez 2 [card] et ajoutez-les à votre main. Glissez ensuite jusqu'à 2 [card] de votre main sous cet oiseau.</t>
+  </si>
+  <si>
+    <t>Vous pouvez glisser entre 0 et 2 carte(s) sous cet oiseau lorsque vous en activez le pouvoir.
+Vous pouvez glisser des cartes que vous aviez déjà en main avant d'en piocher lors de l'activation du pouvoir.</t>
+  </si>
+  <si>
+    <t>Pie-grièche brune</t>
+  </si>
+  <si>
+    <t>Tous les joueurs peuvent stocker 1 [invertebrate] de leur propre réserve sur un oiseau dans leur [grassland]</t>
+  </si>
+  <si>
+    <t>Pour ces pouvoirs, il n'est pas nécessaire que les oiseaux sur lesquels vous stockez de la nourriture aient eux-mêmes des pouvoirs de stockage de nourriture.
+Le nombre de jetons Nourriture à stocker indiqué sur la carte (« sur chaque oiseau de celle ligne » par exemple), est une limite, vous pouvez donc en stocker moins si vous le souhaitez.</t>
+  </si>
+  <si>
+    <t>Pirolle verte</t>
+  </si>
+  <si>
+    <t>Gagnez 1 [invertebrate] ou [rodent] de la mangeoire, si disponible. Vous pouvez le stocker sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Si tous les dés de la mangeoire sont sur la même face, vous pouvez les relancer avant de gagner [nourriture spécifique]. Si la mangeoire ne contient aucun dé avec [nourriture spécifique], vous ne gagnez rien. 
+Lorsqu'un jeton Nourriture est stocké sur une carte Oiseau, vous ne pouvez plus le dépenser. Chaque jeton sur la carte à la fin de la partie vous rapporte 1 point.</t>
+  </si>
+  <si>
+    <t>Iora du Bengale</t>
+  </si>
+  <si>
+    <t>Pondez 1 [egg] sur un autre oiseau dans cette colonne.</t>
+  </si>
+  <si>
+    <t>Martin triste</t>
+  </si>
+  <si>
+    <t>Copiez le pouvoir marron Activation d'un oiseau de la [grassland] du joueur à votre gauche.</t>
+  </si>
+  <si>
+    <t>Chevalier guinette</t>
+  </si>
+  <si>
+    <t>Piochez 1 [card] pour chaque oiseau dans votre [wetland] avec un [egg]. Gardez-en 1 et défaussez le reste.</t>
+  </si>
+  <si>
+    <t>Fauvette couturière</t>
+  </si>
+  <si>
+    <t>Trouvez un groupe d'oiseaux adjacents dans votre réserve avec le même type de nid. Pondez 1 [egg] sur chacun d'entre eux. Les nids [star] comptent comme n'importe quel type de nid.</t>
+  </si>
+  <si>
+    <t>Deux cartes Oiseau sont « adjacentes » si leurs bords se touchent : au-dessus, en dessous, à gauche, ou à droite (les cartes en diagonale ne comptent pas).
+Le groupe peut zigzaguer entre les lignes et les colonnes tant que chaque oiseau du groupe est adjacent à au moins un autre oiseau du groupe.</t>
+  </si>
+  <si>
+    <t>Le pouvoir ainsi copié doit être un pouvoir « Activation ». Résolvez le pouvoir copié comme s'il s'agissait de celui du Martin Triste.</t>
+  </si>
+  <si>
+    <t>Sarcelle d'hiver</t>
+  </si>
+  <si>
+    <t>Pour chaque 3 [egg] dans votre [wetland], piochez 1 [card]. Vous pouvez glisser jusqu'à 2 [card] de votre main sous cet oiseau.</t>
+  </si>
+  <si>
+    <t>Vous pouvez glisser des cartes que vous aviez déjà en main avant d'en piocher lors de l'activation du pouvoir.</t>
+  </si>
+  <si>
+    <t>Barbu à plastron rouge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si tous les dés de la mangeoire sont sur la même face, vous pouvez les relancer avant de gagner [nourriture spécifique]. Si la mangeoire ne contient aucun dé avec [nourriture spécifique], vous ne gagnez rien. </t>
+  </si>
+  <si>
+    <t>Ibis nippon</t>
+  </si>
+  <si>
+    <t>Piochez 2 cartes bonus et gardez-en 1. Les autres joueurs peuvent défausser 2 ressources au choix ([wild], [egg], ou [card]) pour faire de même.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chaque joueur peut défausser 2 ressources identiques (2 [wild] par exemple) ou 2 ressources différentes (par exemple 1 [wild] et 1 [egg]) pour piocher des cartes Bonus.
+Défaussez les [wild] de votre réserve personnelle et les [card] de votre main.
+Piochez 2 cartes Bonus, choisissez celle que vous souhaitez garder et défaussez l'autre. Si la pioche de cartes Bonus est épuisée, mélangez la défausse pour former une nouvelle pioche.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>EXTENSION OCÉANIE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Si un joueur défausse un [nectar] pour piocher ses cartes Bonus, placez le jeton nectar sur la case « nectar dépensé » de son [wetland].</t>
+    </r>
+  </si>
+  <si>
+    <t>Cochevis huppé</t>
+  </si>
+  <si>
+    <t>Défaussez 1 [seed]. Si vous le faites, pondez 1 [egg] sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>La [seed] doit venir de votre réserve. Vous ne pouvez pas en prendre une stockée sur un oiseau.</t>
+  </si>
+  <si>
+    <t>Roselin de Lichtenstein</t>
+  </si>
+  <si>
+    <t>Pondez 1 [egg] sur cet oiseau pour chaque autre oiseau dans votre [grassland].</t>
+  </si>
+  <si>
+    <t>Traquet du désert</t>
+  </si>
+  <si>
+    <t>Pour chaque oiseau dans votre [grassland] avec un [egg], lancez 1 [die]. 
+Choisissez 1 type de nourriture indiqué par un de ces dés et recevez 1 jeton correspondant de la réserve.</t>
+  </si>
+  <si>
+    <t>Vous ne gagnez que 1 jeton Nourriture, quel que soit le nombre de dés lancés.</t>
+  </si>
+  <si>
+    <t>Foulque macroule</t>
+  </si>
+  <si>
+    <t>Glissez jusqu'à 3 [card] de votre main sous cet oiseau.</t>
+  </si>
+  <si>
+    <t>Grand-Duc d'Europe</t>
+  </si>
+  <si>
+    <t>Piochez jusqu'à 3 [card], une par une. Vous pouvez vous arrêter de piocher à tout moment. Lorsque vous vous arrêtez, si l'envergure totale des oiseaux piochés est inférieure à 110cm, glissez-les sous cet oiseau. Sinon, défaussez-les.</t>
+  </si>
+  <si>
+    <t>Ces pouvoirs sont des paris risqués. Après chaque [card] piochée, vérifiez si vous avez réussi ou échoué. Lorsque vous échouez, vous ne pouvez plus piocher de carte, le pouvoir a fini de s'activer. Vous pouvez aussi choisir de vous arrêter et de ne pas piocher de carte à tout moment. Cela vous permet d'éviter d'échouer et de perdre ce que vous auriez gagné.
+Après chaque [card] piochée, additionnez l'envergure de toutes les [card] piochées jusque là. Si le total est supérieur ou égal à 110cm, vous avez échoué. Défaussez toutes les [card] piochées lors de cette activation du pouvoir de cet oiseau.
+Si l'envergure totale est inférieure à 110cm et que vous avez pioché moins de 3 [card] lors de cette activation du pouvoir, vous avez le choix entre piocher une autre [card] ou vous arrêter de piocher et glisser toutes les [card] piochées sous cet oiseau.
+Si vous piochez une [card] avec une envergure variable (comme certains oiseaux de l'extension Océanie), indiqué par un astérisque (*) au lieu de la mesure de l'envergure, vous pouvez choisir n'importe quel nombre positif comme envergure de cet oiseau.</t>
+  </si>
+  <si>
+    <t>Huppe fasciée</t>
+  </si>
+  <si>
+    <t>Volez 1 [invertebrate] à chacun de vos voisins. Chaque voisin à qui vous volez un [invertebrate], peut obtenir 1 [wild] de la réserve.</t>
+  </si>
+  <si>
+    <t>Vous ne pouvez activer ce pouvoir que si l'un de vos voisins possède un [invertebrate]. 
+Dans une partie à 2 joueurs, votre adversaire se trouve à la fois à votre droite et à votre gauche. Comme vous n'avez qu'un seul voisin, vous ne pouvez lui voler que 1 [invertebrate].</t>
+  </si>
+  <si>
+    <t>Faucon crécerelle</t>
+  </si>
+  <si>
+    <t>Lancez 3 [die] au choix. Si vous obtenez au moins 1 [rodent], stockez 1 [rodent] sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Si vous obtenez plus de 1 [rodent], vous n'en stockez tout de même qu'un.</t>
+  </si>
+  <si>
+    <t>Busard des roseaux</t>
+  </si>
+  <si>
+    <t>Grimpereau des bois</t>
+  </si>
+  <si>
+    <t>Pour chaque 3 [egg] dans votre [forest], gagnez 1 [invertebrate] ou [seed] de la réserve. Vous pouvez en stocker jusqu'à 2 sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Comptez les œufs dans l’habitat indiqué, puis divisez le total par 3 arrondis au nombre inférieur. Gagnez autant de jetons Nourriture de la réserve.
+Ces pouvoirs vous donnent le choix entre plusieurs type de nourriture. Si vous gagnez plus d'un jeton, vous pouvez prendre des jetons différents.</t>
+  </si>
+  <si>
+    <t>Serin à front d'or</t>
+  </si>
+  <si>
+    <t>Pondez 1 [egg] sur cet oiseau pour chaque oiseau qui se trouve à sa gauche dans cette ligne.</t>
+  </si>
+  <si>
+    <t>Chevêche forestière</t>
+  </si>
+  <si>
+    <t>Choisissez 2 [die]. Lancez-les jusqu'à 3 fois. A chaque fois, si vous obtenez au moins 1 [invertebrate] ou [rodent], stockez en 1 ici. Sinon, arrêtez de lancer les dés et défaussez toute la nourriture stockée sur l'oiseau lors de ce tour.</t>
+  </si>
+  <si>
+    <t>Faisan doré</t>
+  </si>
+  <si>
+    <t>Tous les joueurs pondent 2 [egg]. Vous pondez 2 [egg] supplémentaires.</t>
+  </si>
+  <si>
+    <t>Chaque joueur peut pondre ses œufs sur le même oiseau ou sur des oiseaux différents.</t>
+  </si>
+  <si>
+    <t>Prinia gracile</t>
+  </si>
+  <si>
+    <t>Défaussez 1 [egg]. Si vous le faites, gagnez 1 [invertebrate] de la réserve.</t>
+  </si>
+  <si>
+    <t>Vous pouvez prendre l'œuf à défausser sur n'importe lequel de vos oiseaux.</t>
+  </si>
+  <si>
+    <t>Grandala bleu</t>
+  </si>
+  <si>
+    <t>Si vous avez pondu un [egg] sur cet oiseau lors de ce tour, glissez 1 [card] de la pioche sous cet oiseau.</t>
+  </si>
+  <si>
+    <t>L'œuf doit avoir été pondu avant d'activer cette carte. Si vous utilisez un autre pouvoir pour copier l'effet du Grandala bleu, vous devez avoir pondu un œuf sur l'oiseau vous permettant de copier le pouvoir à la place.</t>
+  </si>
+  <si>
+    <t>Bergeronnette des ruisseaux</t>
+  </si>
+  <si>
+    <t>Si vous avez utilisé les 4 types d'actions lors de cette manche, gagnez 2 [wild] de la réserve.</t>
+  </si>
+  <si>
+    <t>N'oubliez pas de laisser les cubes Actions dans la colonne de gauche des actions effectuées lors de chaque tour.</t>
+  </si>
+  <si>
+    <t>Grand cormoran</t>
+  </si>
+  <si>
+    <t>Vous pouvez pendre 1 [fish] de cet oiseau, pour le mettre dans votre réserve. Lancez ensuite 2 [die] au choix. Si vous obtenez au moins 1 [fish], stockez 1 [fish] de la réserve sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Calao bicorne</t>
+  </si>
+  <si>
+    <t>Tous les joueurs peuvent glisser une [card] de leur main sous un oiseau dans leur [forest] et/ou stocker 1 [fruit] de leur réserve sur un oiseau dans leur [forest].</t>
+  </si>
+  <si>
+    <t>Outarde à tête noire</t>
+  </si>
+  <si>
+    <t>Marquez immédiatement les points d'une de vos cartes bonus en stockant 1 [seed] de la réserve sur cet oiseau par point gagné. Vous marquerez également les points de la carte normalement à la fin du jeu.</t>
+  </si>
+  <si>
+    <t>Ce pouvoir stocke de la nourriture pour ne pas oublier des points marqués par la carte Bonus lors de son activation. La nourriture ainsi stockée est identique à la nourriture stockée autrement (elle compte par exemple pour la carte Bonus Dissection).</t>
+  </si>
+  <si>
+    <t>Pic épeiche</t>
+  </si>
+  <si>
+    <t>Gagnez 1 [invertebrate] ou [seed] de la mangeoire, si disponible.</t>
+  </si>
+  <si>
+    <t>Marabout argala</t>
+  </si>
+  <si>
+    <t>Copiez le pouvoir d'une des cartes Bonus du joueur à votre gauche (marquez les points en fonction de vos propres oiseaux).</t>
+  </si>
+  <si>
+    <t>Si vous jouez avec les cartes Bonus face cachée et que vous activez ce pouvoir, le joueur indiqué vous montre ses cartes Bonus.
+Lors d'une partie à 2 joueurs, le Vautour indien et le Marabout argala peuvent copier tous les deux la même carte Bonus.</t>
+  </si>
+  <si>
+    <t>Petit guêpier vert</t>
+  </si>
+  <si>
+    <t>Glissez sous cette carte un des oiseaux du plateau qui possèdent [invertebrate] dans leur coût en nourriture, s'il y en a.</t>
+  </si>
+  <si>
+    <t>Faisan versicolore</t>
+  </si>
+  <si>
+    <t>Tous les joueurs pondent 1 [egg].</t>
+  </si>
+  <si>
+    <t>Vous pouvez pondre l'[egg] sur n'importe quel oiseau.</t>
+  </si>
+  <si>
+    <t>Lophophore resplendissant</t>
+  </si>
+  <si>
+    <t>Tous les joueurs gagnent 1 [seed] de la réserve. Pondez également 1 [egg].</t>
+  </si>
+  <si>
+    <t>L'œuf peut être pondu sur n'importe quel oiseau, à condition de ne pas dépasser sa limite d'œufs.</t>
+  </si>
+  <si>
+    <t>Corneille de l'Inde</t>
+  </si>
+  <si>
+    <t>Vous pouvez stocker 1 [wild] de votre réserve sur chaque oiseau de cette ligne.</t>
+  </si>
+  <si>
+    <t>Bec-d'ibis Tibétain</t>
+  </si>
+  <si>
+    <t>Tous les joueurs piochent 1 [card] et gagnent 1 [invertebrate] de la réserve.
+Vous piochez 1 [card] supplémentaire.</t>
+  </si>
+  <si>
+    <t>Paon bleu</t>
+  </si>
+  <si>
+    <t>Tous les joueurs piochent 2 [card]. Vous piochez 1 [card] supplémentaire.</t>
+  </si>
+  <si>
+    <t>Vous pouvez prendre la carte supplémentaire dans la pioche ou sur le plateau Oiseau.</t>
+  </si>
+  <si>
+    <t>Vautour indien</t>
+  </si>
+  <si>
+    <t>Copiez le pouvoir d'une des cartes Bonus du joueur à votre droite (marquez les points en fonction de vos propres oiseaux).</t>
+  </si>
+  <si>
+    <t>Corbeau à gros bec</t>
+  </si>
+  <si>
+    <t>Stockez 1 [wild] de votre réserve sur un oiseau au choix.
+Si vous le faites, vous pouvez glisser 1 [card] de votre main sous cet oiseau.</t>
+  </si>
+  <si>
+    <t>Aigrette garzette</t>
+  </si>
+  <si>
+    <t>Grèbe castagneux</t>
+  </si>
+  <si>
+    <t>Pour chaque oiseau dans cette colonne avec un [egg], piochez 1 [card].
+Gardez-en 1 et défaussez les autres.</t>
+  </si>
+  <si>
+    <t>Petit gravelot</t>
+  </si>
+  <si>
+    <t>Défaussez 1 [card] de votre main. Si vous le faites, pondez 1 [egg] sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Canard mandarin</t>
+  </si>
+  <si>
+    <t>Piochez 5 [card]. Ajoutez-en 1 à votre main, glissez-en 1 sous cet oiseau, donnez-en 1 à un autre joueur et défaussez les autres.</t>
+  </si>
+  <si>
+    <t>Si vous décidez d'activer cet oiseau à la fin de la manche, vous êtes obligé d'effectuer l'ensemble des actions décrites.</t>
+  </si>
+  <si>
+    <t>Souimanga à dos vert</t>
+  </si>
+  <si>
+    <t>Chaque joueur peut lancer 1 [die] au choix et gagner ce jeton Nourriture de la réserve.</t>
+  </si>
+  <si>
+    <t>Chaque joueur peut choisir le même dé ou un dé différent, y compris un dé qui vient d'être lancé par un autre joueur. Ne prenez que le jeton nourriture du dé que vous avez lancé. Si la face obtenue vous donne le choix entre deux jetons Nourriture ([seed]/[invertebrate]), choisissez-en un.</t>
+  </si>
+  <si>
+    <t>Phodile calong</t>
+  </si>
+  <si>
+    <t>Activez les pouvoirs Activation (marron) de tous vos autres [predator].</t>
+  </si>
+  <si>
+    <t>Losque vous utilisez ce pouvoir, vous pouvez activer les pouvoirs Activation (marron) de vos oiseaux [predator] dans l'ordre de votre choix. Ces pouvoirs sont désignés par le symbole [predator] à gauche ou à droite du pouvoir (pas dans le texte du pouvoir).</t>
+  </si>
+  <si>
+    <t>Shama dayal</t>
+  </si>
+  <si>
+    <t>Pour chaque 3 [egg] dans votre [grassland], gagnez 1 [invertebrate] ou [seed] de la réserve.
+Vous pouvez en stocker jusqu'à 2 sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Pithécophage des philippines</t>
+  </si>
+  <si>
+    <t>Lancez les 5 [die]. Vous pouvez relancer autant de [die] que vous les souhaitez, jusqu'à 2 fois. Si vous avez obtenu au moins 3 [rodent] lorsque vous arrêtez de lancer les dés, piochez 2 cartes Bonus de gardez-en 1. Relancez les dés de la mangeoire.</t>
+  </si>
+  <si>
+    <t>Après avoir lancé les 5 dés, vous pouvez en reprendre autant que souhaité pour les relancer (tous en même temps). Vous pouvez répéter à nouveau cette opération (reprendre des dés pour les relancer, tous en même temps). Vous avez donc droit à un total de 3 lancers de dés. Après avoir fini de lancer les dés, si vous avez au moins 3 [rodent] parmi les 5 dés, piochez 2 cartes Bonus et gardez-en 1. Relancez les dés de la mangeoire, quel que soit le nombre de [rodent] parmi les dés.</t>
+  </si>
+  <si>
+    <t>Nymphée fuligineuse</t>
+  </si>
+  <si>
+    <t>Héron pourpré</t>
+  </si>
+  <si>
+    <t>Bengali rouge</t>
+  </si>
+  <si>
+    <t>Coq doré</t>
+  </si>
+  <si>
+    <t>Grue à couronne rouge</t>
+  </si>
+  <si>
+    <t>Bulbul à ventre rouge</t>
+  </si>
+  <si>
+    <t>Vanneau indien</t>
+  </si>
+  <si>
+    <t>Macareux rhinocéros</t>
+  </si>
+  <si>
+    <t>Pigeon biset</t>
+  </si>
+  <si>
+    <t>Corbeau freux</t>
+  </si>
+  <si>
+    <t>Perruche à collier</t>
+  </si>
+  <si>
+    <t>Étourneau roselin</t>
+  </si>
+  <si>
+    <t>Tadorne casarca</t>
+  </si>
+  <si>
+    <t>Grue antigone</t>
+  </si>
+  <si>
+    <t>Tragopan satyre</t>
+  </si>
+  <si>
+    <t>Capucin damier</t>
+  </si>
+  <si>
+    <t>Minivet oranor</t>
+  </si>
+  <si>
+    <t>Harle piette</t>
+  </si>
+  <si>
+    <t>Bécasseau spatule</t>
+  </si>
+  <si>
+    <t>Tourterelle tigrine</t>
+  </si>
+  <si>
+    <t>Pirolle bleue de Ceylan</t>
+  </si>
+  <si>
+    <t>Podarge de Ceylan</t>
+  </si>
+  <si>
+    <t>Martin-chasseur gurial</t>
+  </si>
+  <si>
+    <t>Roselin githagine</t>
+  </si>
+  <si>
+    <t>Linotte à bec jaune</t>
+  </si>
+  <si>
+    <t>Gobemouche vert-de-gris</t>
+  </si>
+  <si>
+    <t>Coucou violet</t>
+  </si>
+  <si>
+    <t>Paruline à sourcils blancs</t>
+  </si>
+  <si>
+    <t>Garrulaxe à huppe blanche</t>
+  </si>
+  <si>
+    <t>Érismature à tête blanche</t>
+  </si>
+  <si>
+    <t>Martin-chasseur à gorge blanche</t>
+  </si>
+  <si>
+    <t>Mésange boréale</t>
+  </si>
+  <si>
+    <t>Blongios de Chine</t>
+  </si>
+  <si>
+    <t>Géopélie zébrée</t>
+  </si>
+  <si>
+    <t>Piochez 1 [card] et ajoutez-la à votre main. Tous les autres joueurs piochent 1 [card]et l'ajoutent à leur main si l'oiseau possède [invertebrate] ou [seed] dans son coût en nourriture.</t>
+  </si>
+  <si>
+    <t>Piochez 1 [card] et ajoutez-la à votre main. Tous les autres joueurs piochent 1 [card] et la gardent si c'est un oiseau de [wetland].</t>
+  </si>
+  <si>
+    <t>L'oiseau doit posséder un symbole [invertebrate] ou [seed]. Le symbole [wild] ne compte pas.</t>
+  </si>
+  <si>
+    <t>Choisissez 2 [die]. Lancez-les jusqu'à 3 fois. A chaque fois, si vous obtenez au moins 1 [invertebrate] ou [fish], stockez en 1 ici. Sinon, arrêtez de lancer les dés et défaussez toute la nourriture stockée sur l'oiseau lors de ce tour.</t>
+  </si>
+  <si>
+    <t>Ce pouvoir est un pari risqué. Après chaque lancer de dé(s), vérifiez si vous avez réussi ou échoué. Lorsque vous échouez, vous ne pouvez plus recommencer, le pouvoir a fini de s activer. Vous pouvez aussi choisir de vous arrêter et de ne pas relancer les dés à tout moment. Cela vous permet d'éviter d'échouer et de perdre ce que vous auriez gagné.
+Si vous échouez, vous devez vous encier et défausser toute la nourriture stockée sur cet oiseau lors de cette activation du pouvoir.
+Si vous réussissez, stockez l nourriture de la reserve sur cet oiseau (ne stockez pas plus d'un jeton après chaque lancer). Si vous avez lancé les dés moins de 3 fois au cours de cette activation du pouvoir, décidez si vous souhaitez les relancer.</t>
+  </si>
+  <si>
+    <t>Donnez 1 [card] de votre main à un autre joueur. Si vous le faites, piochez 2 [card].</t>
+  </si>
+  <si>
+    <t>Comptez les [egg] sur tous vos oiseaux. Si vous avez moins de 6 [egg] au total, pondez 1 [egg] sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Marquez immédiatement les points d'une de vos cartes bonus en stockant 1 [wild] de la réserve sur cet oiseau par point gagné. Défaussez cette carte Bonus et piochez-en une nouvelle.</t>
+  </si>
+  <si>
+    <t>Si vous avez au moins 1 [fruit] dans votre réserve, pondez 1 [egg] sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Défaussez autant de [card] du plateau Oiseaux que vous le souhaitez, puis remplissez-le à nouveau. Si au moins 1 des oiseaux défaussés est un [predator], pondez 1 [egg] sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Lancez 2 [die] au choix. Si vous obtenez au moins 1 [fish], stockez 1 [fish] de la réserve sur cet oiseau. Tous les joueurs peuvent défausser 1 [card] de leur main pour gagner 1 [fish] de la réserve.</t>
+  </si>
+  <si>
+    <t>Tous les joueurs pondent 1 [egg]. Vous pondez 1 [egg] supplémentaire.</t>
+  </si>
+  <si>
+    <t>Stockez 1 [wild] de votre réserve sur cet oiseau ou glissez 1 [card] de votre main sous cette carte. Si vous faites un des deux, glissez 1 [card] de la pioche sous cet oiseau.</t>
+  </si>
+  <si>
+    <t>Copiez un pouvoir Pose (pas de couleur) de 1 des oiseaux de vos voisins.</t>
+  </si>
+  <si>
+    <t>Glissez jusqu'à 3 [card] de votre main sous cet oiseau. Si vous glissez au moins 1 [card], gagnez 1 [invertebrate] de la réserve.</t>
+  </si>
+  <si>
+    <t>Piochez 5 [card]. Ajoutez-en 1 à votre main, glissez-en 1 sous cet oiseau et défaussez les autres.</t>
+  </si>
+  <si>
+    <t>Chaque joueur peut défausser 1 [egg] pour piocher 1 [card].</t>
+  </si>
+  <si>
+    <t>Donnez 1 [card] de votre main à un autre joueur. Si vous le faites, pondez 2 [egg] sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Gagnez 1 [seed] de la réserve ou glissez 1 [card] de la pioche sous cet oiseau.</t>
+  </si>
+  <si>
+    <t>Jouez 1 oiseau supplémentaire dans votre [forest]. Vous pouvez ignorer 1 [invertebrate] ou 1 [egg] dans son coût.</t>
+  </si>
+  <si>
+    <t>Piochez 4 [card]. Glissez 2 [card] sous cette carte, et ajoutez les 2 autres [card] à votre main.</t>
+  </si>
+  <si>
+    <t>Si cet oiseau n'a pas d'oiseaux à sa droite, vous pouvez le déplacer (seulement la carte) sur le plateau du joueur à votre droite (vous choisissez son habitat). Si vous le faites, piochez 3 [card].</t>
+  </si>
+  <si>
+    <t>Vous pouvez stocker 1 [wild] de votre réserve sur chacun de vos autres oiseaux.</t>
+  </si>
+  <si>
+    <t>Lancez 1 [die] au choix. Si vous obtenez un [invertabrate], stockez 1 [invertebrate] de la réserve sur cet oiseau. Tous les joueurs peuvent défausser 1 [card] de leur main pour gagner 1 [invertebrate] de la réserve.</t>
+  </si>
+  <si>
+    <t>Choisissez 1 [die]. Lancez-le une fois pour chacun de vos oiseaux [wetland].
+Si vous obtenez au moins 1 [fish], gagnez-en 1 de la réserve. Vous pouvez le stocker sur cet oiseau.</t>
+  </si>
+  <si>
+    <t>Jouez un oiseau supplémentaire dans votre [grassland]. Vous pouvez ignorer 1 [seed] ou 1 [egg] dans son coût.</t>
+  </si>
+  <si>
+    <t>Piochez 2 [card] et ajoutez-les à votre main. Glissez ensuite  2 [card] de votre main sous cet oiseau.</t>
+  </si>
+  <si>
+    <t>Si vous avez gagné un [invertebrate] de la mangeoire lors de ce tour, gagnez 1 [fruit] de la réserve.</t>
+  </si>
+  <si>
+    <t>Lorsqu'un autre joueur effectue l'action Pondre des œufs, vous pouvez pondre 1 [egg] sur un oiseau d'envergure inférieure à 30cm. Ce pouvoir vous permet de pondre 2 œufs de plus que la limite habituelle.</t>
+  </si>
+  <si>
+    <t>Pour chaque oiseau dans votre [forest] avec un œuf dessus, lancez 1 [die] au choix. Choisissez 1 type de nourriture indiqué par un de ces dés et recevez un jeton correspondant de la réserve.</t>
+  </si>
+  <si>
+    <t>Glissez 1 [card] de votre main sous cet oiseau. Si vous le faites, gagnez 1 [invertebrate], [seed], ou [fruit] de la mangeoire.</t>
+  </si>
+  <si>
+    <t>Piochez 3 cartes Bonus et gardez-en 1.</t>
+  </si>
+  <si>
+    <t>Choisissez 1 [die]. Lancez-le jusqu'à 3 fois. A chaque fois, si vous obtenez [invertebrate], [fish], ou [rodent] stockez en 1 ici. Sinon, arrêtez de lancer les dés et défaussez toute la nourriture stockée sur l'oiseau lors de ce tour.</t>
+  </si>
+  <si>
+    <t>Stockez sur cet oiseau 1 [invertebrate], [seed], ou [fruit] de la mangeoire, si disponible.</t>
+  </si>
+  <si>
+    <t>Piochez la [card] du milieu sur le plateau Oiseaux.</t>
+  </si>
+  <si>
+    <t>Tous les joueurs peuvent défausser 1 [seed] de leur réserve pour pondre 1 [egg].</t>
+  </si>
+  <si>
+    <t>Amateur d'espèces rares [automa]</t>
+  </si>
+  <si>
+    <t>Ne défaussez pas la [fruit].</t>
+  </si>
+  <si>
+    <t>La face ([invertebrate]/[seed]) compte comme si vous aviez obtenu un [invertebrate].
+Lorsque vous lancez 2 dés, vous ne pouvez stocker que 1 [fish], même si vous obtenez 2 [fish] aux dés.
+La seconde partie de ce pouvoir est indépendante de la première. Tous les joueurs peuvent défausser une [card] pour gagner de la nourriture, et ce quel que soit le résultat du lancer de dés. Les consignes « tous les joueurs » s'appliquent à vous aussi.</t>
+  </si>
+  <si>
+    <t>Vous pouvez pondre l'[egg] sur n'importe quel oiseau. Vous pouvez pondre le deuxième œuf sur le même oiseau que le premier (mais ce n'est pas obligatoire).</t>
+  </si>
+  <si>
+    <t>Le pouvoir ainsi copié doit être un pouvoir « Pose » (pas de couleur).
+Cet oiseau peut copier un pouvoir « Pose » qui vous permet de jouer un oiseau supplémentaire, même dans un autre habitat que celui dans lequel vous avez joué cet oiseau. L'oiseau supplémentaire doit être joué dans l'habitat indiqué par le pouvoir copié, s'il y en a un.
+Comme cet oiseau ne peut pas être joué dans le [wetland], il ne peut pas copier un pouvoir « Pose » spécifiant de jouer l'oiseau dans cet habitat (par exemple le Héron Cendré de l'extension Europe).
+Si vous utilisez cet oiseau pour copier le pouvoir « Pose » d'un oiseau avec un coût alternatif de nourriture, vous pouvez payer ce coût alternatif pour jouer cet oiseau, comme indiqué dans le pouvoir. (Aucun oiseau de cette extension n'a de coût alternatif, mais c'est le cas de certains oiseaux de l'extension Europe. Ces coûts alternatifs sont indiqués par un astérisque [*] à côté du coût en nourriture.)</t>
+  </si>
+  <si>
+    <t>Pour ce pouvoir, il n'est pas nécessaire que les oiseaux sur lesquels vous stockez de la nourriture aient eux-mêmes des pouvoirs de stockage de nourriture.
+Le nombre de jetons Nourriture à stocker indiqué sur la carte (« sur chaque oiseau de celle ligne » par exemple), est une limite, vous pouvez donc en stocker moins si vous le souhaitez.</t>
+  </si>
+  <si>
+    <t>Vous pouvez ignorer un symbole [wild] dans le coût en nourriture de l'oiseau au lieu d'ignorer 1 [invertebrate].</t>
+  </si>
+  <si>
+    <t>Lorsque vous utilisez le pouvoir de cet oiseau, vous êtes obligé de glisser les cartes sous celui-ci.</t>
+  </si>
+  <si>
+    <t>Chaque joueur peut défausser 2 ressources identiques (2 [wild] par exemple) ou 2 ressources différentes (par exemple 1 [wild] et 1 [egg]) pour piocher des cartes Bonus.
+Défaussez les [wild] de votre réserve personnelle et les [card] de votre main.
+Piochez 2 cartes Bonus, choisissez celle que vous souhaitez garder et défaussez l'autre. Si la pioche de cartes Bonus est épuisée, mélangez la défausse pour former une nouvelle pioche.
+EXTENSION OCÉANIE Si un joueur défausse un [nectar] pour piocher ses cartes Bonus, placez le jeton nectar sur la case « nectar dépensé » de son [wetland].</t>
+  </si>
+  <si>
+    <t>Si vous gagnez plus de 1 [fish], vous n'en gardez tout de même qu'un.</t>
+  </si>
+  <si>
+    <t>Vous pouvez ignorer un symbole [wild] dans le coût en nourriture de l'oiseau au lieu d'ignorer 1 [seed].</t>
+  </si>
+  <si>
+    <t>Lorsque vous utilisez le pouvoir de cet oiseau, vous êtes obligé de glisser les cartes sous celui-ci.
+Vous pouvez glisser des cartes que vous aviez déjà en main avant d'en piocher lors de l'activation du pouvoir.</t>
+  </si>
+  <si>
+    <t>Vous pouvez appliquer ce pouvoir aux [invertebrate] gagnés avant ou après avoir activé le Gobemouche vert-de-gris. Cpendant vous ne pouvez utiliser ce pouvoir qu'une seule fois par tour, et donc gagner un seul [fruit] quel que soit le nombre de [invertebrate] gagnés.</t>
+  </si>
+  <si>
+    <t>Si tous les dés de la mangeoire sont sur la même face, vous pouvez les relancer avant de gagner [nourriture spécifique]. Si la mangeoire ne contient aucun dé avec [nourriture spécifique], vous ne gagnez rien.</t>
+  </si>
+  <si>
+    <t>Piochez 3 cartes Bonus, choisissez celle que vous souhaitez garder et défaussez les autres. Si la pioche de cartes Bonus est épuisée, mélangez la défausse pour former une nouvelle pioche.</t>
+  </si>
+  <si>
+    <t>N'oubliez pas : les cartes du plateau ne doivent jamais être déplacées (que ce soit vers la droite ou vers la gauche) lorsque vous en piochez une. Si l'emplacement du milieu est vide, ce pouvoir ne s'active pas.</t>
+  </si>
+  <si>
+    <t>Si vous défaussez un [seed], vous pouvez pondre l'[egg] sur n'importe quel oiseau, pas forcément sur la Géopélie zébrée.</t>
+  </si>
 </sst>
 </file>
 
@@ -5658,7 +6397,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;PRAWDA&quot;;&quot;PRAWDA&quot;;&quot;FAŁSZ&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5701,6 +6440,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -6033,22 +6779,26 @@
   <dimension ref="A1:K447"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C174" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C443" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A219" sqref="A219"/>
-      <selection pane="bottomRight" activeCell="F178" sqref="F178"/>
+      <selection pane="bottomRight" activeCell="F444" sqref="F444"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.86328125" customWidth="1"/>
-    <col min="3" max="3" width="26.1328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.86328125" customWidth="1"/>
-    <col min="5" max="5" width="26.1328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.73046875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="54.1328125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="4.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="54.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13.5" customHeight="1">
@@ -15855,7 +16605,7 @@
       <c r="J357" s="3"/>
       <c r="K357" s="3"/>
     </row>
-    <row r="358" spans="1:11">
+    <row r="358" spans="1:11" ht="30">
       <c r="A358" s="1">
         <v>358</v>
       </c>
@@ -15868,8 +16618,14 @@
       <c r="D358" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="359" spans="1:11">
+      <c r="E358" s="1" t="s">
+        <v>1833</v>
+      </c>
+      <c r="F358" s="2" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="359" spans="1:11" ht="150">
       <c r="A359" s="1">
         <v>359</v>
       </c>
@@ -15882,8 +16638,17 @@
       <c r="D359" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="360" spans="1:11">
+      <c r="E359" s="1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="F359" s="2" t="s">
+        <v>1828</v>
+      </c>
+      <c r="G359" s="2" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="360" spans="1:11" ht="30">
       <c r="A360" s="1">
         <v>360</v>
       </c>
@@ -15896,8 +16661,17 @@
       <c r="D360" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="361" spans="1:11">
+      <c r="E360" s="1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="F360" s="2" t="s">
+        <v>1830</v>
+      </c>
+      <c r="K360" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="361" spans="1:11" ht="45">
       <c r="A361" s="1">
         <v>361</v>
       </c>
@@ -15910,8 +16684,14 @@
       <c r="D361" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="362" spans="1:11">
+      <c r="E361" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="F361" s="2" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="362" spans="1:11" ht="45">
       <c r="A362" s="1">
         <v>362</v>
       </c>
@@ -15924,8 +16704,14 @@
       <c r="D362" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="363" spans="1:11">
+      <c r="E362" s="1" t="s">
+        <v>1837</v>
+      </c>
+      <c r="F362" s="2" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="363" spans="1:11" ht="75">
       <c r="A363" s="1">
         <v>363</v>
       </c>
@@ -15938,8 +16724,20 @@
       <c r="D363" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="364" spans="1:11">
+      <c r="E363" s="2" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F363" s="2" t="s">
+        <v>1841</v>
+      </c>
+      <c r="G363" s="2" t="s">
+        <v>1842</v>
+      </c>
+      <c r="K363" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="364" spans="1:11" ht="30">
       <c r="A364" s="1">
         <v>364</v>
       </c>
@@ -15952,8 +16750,17 @@
       <c r="D364" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="365" spans="1:11">
+      <c r="E364" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="F364" s="2" t="s">
+        <v>1832</v>
+      </c>
+      <c r="K364" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="365" spans="1:11" ht="60">
       <c r="A365" s="1">
         <v>365</v>
       </c>
@@ -15966,8 +16773,23 @@
       <c r="D365" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="366" spans="1:11">
+      <c r="E365" s="1" t="s">
+        <v>1843</v>
+      </c>
+      <c r="F365" s="2" t="s">
+        <v>1844</v>
+      </c>
+      <c r="G365" s="2" t="s">
+        <v>1845</v>
+      </c>
+      <c r="I365" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K365" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="366" spans="1:11" ht="105">
       <c r="A366" s="1">
         <v>366</v>
       </c>
@@ -15980,8 +16802,20 @@
       <c r="D366" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="367" spans="1:11">
+      <c r="E366" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="F366" s="2" t="s">
+        <v>1847</v>
+      </c>
+      <c r="G366" s="2" t="s">
+        <v>1848</v>
+      </c>
+      <c r="K366" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="367" spans="1:11" ht="225">
       <c r="A367" s="1">
         <v>367</v>
       </c>
@@ -15994,8 +16828,20 @@
       <c r="D367" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="368" spans="1:11">
+      <c r="E367" s="1" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F367" s="2" t="s">
+        <v>1850</v>
+      </c>
+      <c r="G367" s="2" t="s">
+        <v>1851</v>
+      </c>
+      <c r="K367" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="368" spans="1:11" ht="75">
       <c r="A368" s="1">
         <v>368</v>
       </c>
@@ -16008,8 +16854,20 @@
       <c r="D368" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="369" spans="1:4">
+      <c r="E368" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="F368" s="2" t="s">
+        <v>1853</v>
+      </c>
+      <c r="G368" s="2" t="s">
+        <v>1854</v>
+      </c>
+      <c r="I368" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="369" spans="1:11" ht="120">
       <c r="A369" s="1">
         <v>369</v>
       </c>
@@ -16022,8 +16880,20 @@
       <c r="D369" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="370" spans="1:4">
+      <c r="E369" s="1" t="s">
+        <v>1855</v>
+      </c>
+      <c r="F369" s="2" t="s">
+        <v>1856</v>
+      </c>
+      <c r="G369" s="2" t="s">
+        <v>1857</v>
+      </c>
+      <c r="K369" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" ht="105">
       <c r="A370" s="1">
         <v>370</v>
       </c>
@@ -16036,8 +16906,20 @@
       <c r="D370" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="371" spans="1:4">
+      <c r="E370" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="F370" s="2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="G370" s="2" t="s">
+        <v>1860</v>
+      </c>
+      <c r="K370" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="371" spans="1:11" ht="30">
       <c r="A371" s="1">
         <v>371</v>
       </c>
@@ -16050,8 +16932,17 @@
       <c r="D371" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="372" spans="1:4">
+      <c r="E371" s="1" t="s">
+        <v>1861</v>
+      </c>
+      <c r="F371" s="2" t="s">
+        <v>1862</v>
+      </c>
+      <c r="I371" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" ht="45">
       <c r="A372" s="1">
         <v>372</v>
       </c>
@@ -16064,8 +16955,17 @@
       <c r="D372" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="373" spans="1:4">
+      <c r="E372" s="1" t="s">
+        <v>1863</v>
+      </c>
+      <c r="F372" s="2" t="s">
+        <v>1864</v>
+      </c>
+      <c r="G372" s="2" t="s">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" ht="45">
       <c r="A373" s="1">
         <v>373</v>
       </c>
@@ -16078,8 +16978,14 @@
       <c r="D373" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="374" spans="1:4">
+      <c r="E373" s="1" t="s">
+        <v>1865</v>
+      </c>
+      <c r="F373" s="2" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" ht="90">
       <c r="A374" s="1">
         <v>374</v>
       </c>
@@ -16092,8 +16998,17 @@
       <c r="D374" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="375" spans="1:4">
+      <c r="E374" s="1" t="s">
+        <v>1867</v>
+      </c>
+      <c r="F374" s="2" t="s">
+        <v>1868</v>
+      </c>
+      <c r="G374" s="2" t="s">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11" ht="45">
       <c r="A375" s="1">
         <v>375</v>
       </c>
@@ -16106,8 +17021,17 @@
       <c r="D375" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="376" spans="1:4">
+      <c r="E375" s="1" t="s">
+        <v>1871</v>
+      </c>
+      <c r="F375" s="2" t="s">
+        <v>1872</v>
+      </c>
+      <c r="G375" s="2" t="s">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="376" spans="1:11" ht="60">
       <c r="A376" s="1">
         <v>376</v>
       </c>
@@ -16120,8 +17044,23 @@
       <c r="D376" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="377" spans="1:4">
+      <c r="E376" s="1" t="s">
+        <v>1874</v>
+      </c>
+      <c r="F376" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="G376" s="2" t="s">
+        <v>1875</v>
+      </c>
+      <c r="H376" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K376" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="377" spans="1:11" ht="210">
       <c r="A377" s="1">
         <v>377</v>
       </c>
@@ -16134,8 +17073,20 @@
       <c r="D377" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="378" spans="1:4">
+      <c r="E377" s="1" t="s">
+        <v>1876</v>
+      </c>
+      <c r="F377" s="2" t="s">
+        <v>1877</v>
+      </c>
+      <c r="G377" s="2" t="s">
+        <v>1878</v>
+      </c>
+      <c r="I377" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="378" spans="1:11" ht="30">
       <c r="A378" s="1">
         <v>378</v>
       </c>
@@ -16148,8 +17099,20 @@
       <c r="D378" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="379" spans="1:4">
+      <c r="E378" s="1" t="s">
+        <v>1879</v>
+      </c>
+      <c r="F378" s="2" t="s">
+        <v>1880</v>
+      </c>
+      <c r="G378" s="2" t="s">
+        <v>1881</v>
+      </c>
+      <c r="H378" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="379" spans="1:11" ht="30">
       <c r="A379" s="1">
         <v>379</v>
       </c>
@@ -16162,8 +17125,17 @@
       <c r="D379" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="380" spans="1:4">
+      <c r="E379" s="1" t="s">
+        <v>1882</v>
+      </c>
+      <c r="F379" s="2" t="s">
+        <v>1883</v>
+      </c>
+      <c r="I379" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="380" spans="1:11" ht="75">
       <c r="A380" s="1">
         <v>380</v>
       </c>
@@ -16176,8 +17148,20 @@
       <c r="D380" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="381" spans="1:4">
+      <c r="E380" s="1" t="s">
+        <v>1884</v>
+      </c>
+      <c r="F380" s="2" t="s">
+        <v>1885</v>
+      </c>
+      <c r="G380" s="2" t="s">
+        <v>1886</v>
+      </c>
+      <c r="I380" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" ht="30">
       <c r="A381" s="1">
         <v>381</v>
       </c>
@@ -16190,8 +17174,14 @@
       <c r="D381" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="382" spans="1:4">
+      <c r="E381" s="1" t="s">
+        <v>1887</v>
+      </c>
+      <c r="F381" s="2" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11" ht="375">
       <c r="A382" s="1">
         <v>382</v>
       </c>
@@ -16204,8 +17194,20 @@
       <c r="D382" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="383" spans="1:4">
+      <c r="E382" s="1" t="s">
+        <v>1889</v>
+      </c>
+      <c r="F382" s="2" t="s">
+        <v>1890</v>
+      </c>
+      <c r="G382" s="2" t="s">
+        <v>1891</v>
+      </c>
+      <c r="I382" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="383" spans="1:11" ht="105">
       <c r="A383" s="1">
         <v>383</v>
       </c>
@@ -16218,8 +17220,17 @@
       <c r="D383" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="384" spans="1:4">
+      <c r="E383" s="1" t="s">
+        <v>1892</v>
+      </c>
+      <c r="F383" s="2" t="s">
+        <v>1893</v>
+      </c>
+      <c r="G383" s="2" t="s">
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" ht="45">
       <c r="A384" s="1">
         <v>384</v>
       </c>
@@ -16232,8 +17243,17 @@
       <c r="D384" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="385" spans="1:4">
+      <c r="E384" s="1" t="s">
+        <v>1895</v>
+      </c>
+      <c r="F384" s="2" t="s">
+        <v>1896</v>
+      </c>
+      <c r="G384" s="2" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="385" spans="1:11" ht="375">
       <c r="A385" s="1">
         <v>385</v>
       </c>
@@ -16246,8 +17266,20 @@
       <c r="D385" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="386" spans="1:4">
+      <c r="E385" s="1" t="s">
+        <v>1898</v>
+      </c>
+      <c r="F385" s="2" t="s">
+        <v>1890</v>
+      </c>
+      <c r="G385" s="2" t="s">
+        <v>1891</v>
+      </c>
+      <c r="I385" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="386" spans="1:11" ht="105">
       <c r="A386" s="1">
         <v>386</v>
       </c>
@@ -16260,8 +17292,20 @@
       <c r="D386" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="387" spans="1:4">
+      <c r="E386" s="1" t="s">
+        <v>1899</v>
+      </c>
+      <c r="F386" s="2" t="s">
+        <v>1900</v>
+      </c>
+      <c r="G386" s="2" t="s">
+        <v>1901</v>
+      </c>
+      <c r="I386" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="387" spans="1:11" ht="45">
       <c r="A387" s="1">
         <v>387</v>
       </c>
@@ -16274,8 +17318,20 @@
       <c r="D387" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="388" spans="1:4">
+      <c r="E387" s="1" t="s">
+        <v>1902</v>
+      </c>
+      <c r="F387" s="2" t="s">
+        <v>1903</v>
+      </c>
+      <c r="H387" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K387" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="388" spans="1:11" ht="225">
       <c r="A388" s="1">
         <v>388</v>
       </c>
@@ -16288,8 +17344,17 @@
       <c r="D388" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="389" spans="1:4">
+      <c r="E388" s="1" t="s">
+        <v>1904</v>
+      </c>
+      <c r="F388" s="2" t="s">
+        <v>1905</v>
+      </c>
+      <c r="G388" s="2" t="s">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="389" spans="1:11" ht="30">
       <c r="A389" s="1">
         <v>389</v>
       </c>
@@ -16302,8 +17367,20 @@
       <c r="D389" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="390" spans="1:4">
+      <c r="E389" s="1" t="s">
+        <v>1906</v>
+      </c>
+      <c r="F389" s="2" t="s">
+        <v>1907</v>
+      </c>
+      <c r="G389" s="2" t="s">
+        <v>1908</v>
+      </c>
+      <c r="K389" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="390" spans="1:11" ht="30">
       <c r="A390" s="1">
         <v>390</v>
       </c>
@@ -16316,8 +17393,17 @@
       <c r="D390" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="391" spans="1:4">
+      <c r="E390" s="1" t="s">
+        <v>1909</v>
+      </c>
+      <c r="F390" s="2" t="s">
+        <v>1910</v>
+      </c>
+      <c r="G390" s="2" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="391" spans="1:11" ht="60">
       <c r="A391" s="1">
         <v>391</v>
       </c>
@@ -16330,8 +17416,20 @@
       <c r="D391" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="392" spans="1:4">
+      <c r="E391" s="1" t="s">
+        <v>1912</v>
+      </c>
+      <c r="F391" s="2" t="s">
+        <v>1913</v>
+      </c>
+      <c r="G391" s="2" t="s">
+        <v>1914</v>
+      </c>
+      <c r="K391" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="392" spans="1:11" ht="30">
       <c r="A392" s="1">
         <v>392</v>
       </c>
@@ -16344,8 +17442,20 @@
       <c r="D392" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="393" spans="1:4">
+      <c r="E392" s="1" t="s">
+        <v>1915</v>
+      </c>
+      <c r="F392" s="2" t="s">
+        <v>1916</v>
+      </c>
+      <c r="G392" s="2" t="s">
+        <v>1917</v>
+      </c>
+      <c r="I392" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="393" spans="1:11" ht="75">
       <c r="A393" s="1">
         <v>393</v>
       </c>
@@ -16358,8 +17468,14 @@
       <c r="D393" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="394" spans="1:4">
+      <c r="E393" s="1" t="s">
+        <v>1918</v>
+      </c>
+      <c r="F393" s="2" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="394" spans="1:11" ht="60">
       <c r="A394" s="1">
         <v>394</v>
       </c>
@@ -16372,8 +17488,17 @@
       <c r="D394" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="395" spans="1:4">
+      <c r="E394" s="1" t="s">
+        <v>1920</v>
+      </c>
+      <c r="F394" s="2" t="s">
+        <v>1921</v>
+      </c>
+      <c r="H394" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="395" spans="1:11" ht="75">
       <c r="A395" s="1">
         <v>395</v>
       </c>
@@ -16386,8 +17511,23 @@
       <c r="D395" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="396" spans="1:4">
+      <c r="E395" s="1" t="s">
+        <v>1922</v>
+      </c>
+      <c r="F395" s="2" t="s">
+        <v>1923</v>
+      </c>
+      <c r="G395" s="2" t="s">
+        <v>1924</v>
+      </c>
+      <c r="H395" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K395" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="396" spans="1:11" ht="60">
       <c r="A396" s="1">
         <v>396</v>
       </c>
@@ -16400,8 +17540,17 @@
       <c r="D396" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="397" spans="1:4">
+      <c r="E396" s="1" t="s">
+        <v>1925</v>
+      </c>
+      <c r="F396" s="2" t="s">
+        <v>1926</v>
+      </c>
+      <c r="G396" s="2" t="s">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="397" spans="1:11" ht="105">
       <c r="A397" s="1">
         <v>397</v>
       </c>
@@ -16414,8 +17563,17 @@
       <c r="D397" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="398" spans="1:4">
+      <c r="E397" s="1" t="s">
+        <v>1927</v>
+      </c>
+      <c r="F397" s="2" t="s">
+        <v>1928</v>
+      </c>
+      <c r="G397" s="2" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="398" spans="1:11" ht="45">
       <c r="A398" s="1">
         <v>398</v>
       </c>
@@ -16428,8 +17586,17 @@
       <c r="D398" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="399" spans="1:4">
+      <c r="E398" s="1" t="s">
+        <v>1930</v>
+      </c>
+      <c r="F398" s="2" t="s">
+        <v>1931</v>
+      </c>
+      <c r="K398" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="399" spans="1:11">
       <c r="A399" s="1">
         <v>399</v>
       </c>
@@ -16442,8 +17609,20 @@
       <c r="D399" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="400" spans="1:4">
+      <c r="E399" s="1" t="s">
+        <v>1932</v>
+      </c>
+      <c r="F399" s="2" t="s">
+        <v>1933</v>
+      </c>
+      <c r="G399" s="2" t="s">
+        <v>1934</v>
+      </c>
+      <c r="K399" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="400" spans="1:11" ht="30">
       <c r="A400" s="1">
         <v>400</v>
       </c>
@@ -16456,8 +17635,17 @@
       <c r="D400" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="401" spans="1:4">
+      <c r="E400" s="1" t="s">
+        <v>1935</v>
+      </c>
+      <c r="F400" s="2" t="s">
+        <v>1936</v>
+      </c>
+      <c r="G400" s="2" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="401" spans="1:11" ht="120">
       <c r="A401" s="1">
         <v>401</v>
       </c>
@@ -16470,8 +17658,20 @@
       <c r="D401" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="402" spans="1:4">
+      <c r="E401" s="1" t="s">
+        <v>1938</v>
+      </c>
+      <c r="F401" s="2" t="s">
+        <v>1939</v>
+      </c>
+      <c r="G401" s="2" t="s">
+        <v>2043</v>
+      </c>
+      <c r="I401" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="402" spans="1:11" ht="45">
       <c r="A402" s="1">
         <v>402</v>
       </c>
@@ -16484,8 +17684,20 @@
       <c r="D402" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="403" spans="1:4">
+      <c r="E402" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="F402" s="2" t="s">
+        <v>1941</v>
+      </c>
+      <c r="H402" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I402" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" ht="30">
       <c r="A403" s="1">
         <v>403</v>
       </c>
@@ -16498,8 +17710,20 @@
       <c r="D403" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="404" spans="1:4">
+      <c r="E403" s="1" t="s">
+        <v>1942</v>
+      </c>
+      <c r="F403" s="2" t="s">
+        <v>1943</v>
+      </c>
+      <c r="G403" s="2" t="s">
+        <v>1944</v>
+      </c>
+      <c r="K403" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="404" spans="1:11" ht="105">
       <c r="A404" s="1">
         <v>404</v>
       </c>
@@ -16512,8 +17736,20 @@
       <c r="D404" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="405" spans="1:4">
+      <c r="E404" s="1" t="s">
+        <v>1945</v>
+      </c>
+      <c r="F404" s="2" t="s">
+        <v>1946</v>
+      </c>
+      <c r="G404" s="2" t="s">
+        <v>1929</v>
+      </c>
+      <c r="I404" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="405" spans="1:11" ht="120">
       <c r="A405" s="1">
         <v>405</v>
       </c>
@@ -16526,8 +17762,20 @@
       <c r="D405" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="406" spans="1:4">
+      <c r="E405" s="1" t="s">
+        <v>1947</v>
+      </c>
+      <c r="F405" s="2" t="s">
+        <v>1948</v>
+      </c>
+      <c r="G405" s="2" t="s">
+        <v>2043</v>
+      </c>
+      <c r="H405" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="406" spans="1:11" ht="45">
       <c r="A406" s="1">
         <v>406</v>
       </c>
@@ -16540,8 +17788,14 @@
       <c r="D406" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="407" spans="1:4">
+      <c r="E406" s="1" t="s">
+        <v>1949</v>
+      </c>
+      <c r="F406" s="2" t="s">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="407" spans="1:11" ht="45">
       <c r="A407" s="1">
         <v>407</v>
       </c>
@@ -16554,8 +17808,14 @@
       <c r="D407" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="408" spans="1:4">
+      <c r="E407" s="1" t="s">
+        <v>1950</v>
+      </c>
+      <c r="F407" s="2" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="408" spans="1:11" ht="30">
       <c r="A408" s="1">
         <v>408</v>
       </c>
@@ -16568,8 +17828,14 @@
       <c r="D408" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="409" spans="1:4">
+      <c r="E408" s="1" t="s">
+        <v>1952</v>
+      </c>
+      <c r="F408" s="2" t="s">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="409" spans="1:11" ht="45">
       <c r="A409" s="1">
         <v>409</v>
       </c>
@@ -16582,8 +17848,17 @@
       <c r="D409" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="410" spans="1:4">
+      <c r="E409" s="1" t="s">
+        <v>1954</v>
+      </c>
+      <c r="F409" s="2" t="s">
+        <v>1955</v>
+      </c>
+      <c r="G409" s="2" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="410" spans="1:11" ht="90">
       <c r="A410" s="1">
         <v>410</v>
       </c>
@@ -16596,8 +17871,23 @@
       <c r="D410" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="411" spans="1:4">
+      <c r="E410" s="1" t="s">
+        <v>1957</v>
+      </c>
+      <c r="F410" s="2" t="s">
+        <v>1958</v>
+      </c>
+      <c r="G410" s="2" t="s">
+        <v>1959</v>
+      </c>
+      <c r="H410" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K410" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" ht="75">
       <c r="A411" s="1">
         <v>411</v>
       </c>
@@ -16610,8 +17900,17 @@
       <c r="D411" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="412" spans="1:4">
+      <c r="E411" s="1" t="s">
+        <v>1960</v>
+      </c>
+      <c r="F411" s="2" t="s">
+        <v>1961</v>
+      </c>
+      <c r="G411" s="2" t="s">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="412" spans="1:11" ht="105">
       <c r="A412" s="1">
         <v>412</v>
       </c>
@@ -16624,8 +17923,17 @@
       <c r="D412" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="413" spans="1:4">
+      <c r="E412" s="1" t="s">
+        <v>1963</v>
+      </c>
+      <c r="F412" s="2" t="s">
+        <v>1964</v>
+      </c>
+      <c r="G412" s="2" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="413" spans="1:11" ht="135">
       <c r="A413" s="1">
         <v>413</v>
       </c>
@@ -16638,8 +17946,20 @@
       <c r="D413" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="414" spans="1:4">
+      <c r="E413" s="1" t="s">
+        <v>1965</v>
+      </c>
+      <c r="F413" s="2" t="s">
+        <v>1966</v>
+      </c>
+      <c r="G413" s="2" t="s">
+        <v>1967</v>
+      </c>
+      <c r="I413" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="414" spans="1:11" ht="75">
       <c r="A414" s="1">
         <v>414</v>
       </c>
@@ -16652,8 +17972,17 @@
       <c r="D414" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="415" spans="1:4">
+      <c r="E414" s="1" t="s">
+        <v>1968</v>
+      </c>
+      <c r="F414" s="2" t="s">
+        <v>2002</v>
+      </c>
+      <c r="G414" s="2" t="s">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="415" spans="1:11" ht="225">
       <c r="A415" s="1">
         <v>415</v>
       </c>
@@ -16666,8 +17995,20 @@
       <c r="D415" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="416" spans="1:4">
+      <c r="E415" s="1" t="s">
+        <v>1969</v>
+      </c>
+      <c r="F415" s="2" t="s">
+        <v>2005</v>
+      </c>
+      <c r="G415" s="2" t="s">
+        <v>2006</v>
+      </c>
+      <c r="K415" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="416" spans="1:11" ht="30">
       <c r="A416" s="1">
         <v>416</v>
       </c>
@@ -16680,8 +18021,17 @@
       <c r="D416" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="417" spans="1:4">
+      <c r="E416" s="1" t="s">
+        <v>1970</v>
+      </c>
+      <c r="F416" s="2" t="s">
+        <v>2007</v>
+      </c>
+      <c r="K416" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="417" spans="1:11" ht="45">
       <c r="A417" s="1">
         <v>417</v>
       </c>
@@ -16694,8 +18044,17 @@
       <c r="D417" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="418" spans="1:4">
+      <c r="E417" s="1" t="s">
+        <v>1971</v>
+      </c>
+      <c r="F417" s="2" t="s">
+        <v>2008</v>
+      </c>
+      <c r="K417" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="418" spans="1:11" ht="75">
       <c r="A418" s="1">
         <v>418</v>
       </c>
@@ -16708,8 +18067,23 @@
       <c r="D418" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="419" spans="1:4">
+      <c r="E418" s="1" t="s">
+        <v>1972</v>
+      </c>
+      <c r="F418" s="2" t="s">
+        <v>2009</v>
+      </c>
+      <c r="G418" s="2" t="s">
+        <v>1924</v>
+      </c>
+      <c r="H418" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K418" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="419" spans="1:11" ht="30">
       <c r="A419" s="1">
         <v>419</v>
       </c>
@@ -16722,8 +18096,23 @@
       <c r="D419" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="420" spans="1:4">
+      <c r="E419" s="1" t="s">
+        <v>1973</v>
+      </c>
+      <c r="F419" s="2" t="s">
+        <v>2010</v>
+      </c>
+      <c r="G419" s="2" t="s">
+        <v>2039</v>
+      </c>
+      <c r="H419" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K419" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="420" spans="1:11" ht="75">
       <c r="A420" s="1">
         <v>420</v>
       </c>
@@ -16736,8 +18125,17 @@
       <c r="D420" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="421" spans="1:4">
+      <c r="E420" s="1" t="s">
+        <v>1974</v>
+      </c>
+      <c r="F420" s="2" t="s">
+        <v>2011</v>
+      </c>
+      <c r="I420" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="421" spans="1:11" ht="165">
       <c r="A421" s="1">
         <v>421</v>
       </c>
@@ -16750,8 +18148,17 @@
       <c r="D421" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="422" spans="1:4">
+      <c r="E421" s="1" t="s">
+        <v>1975</v>
+      </c>
+      <c r="F421" s="2" t="s">
+        <v>2012</v>
+      </c>
+      <c r="G421" s="2" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="422" spans="1:11" ht="45">
       <c r="A422" s="1">
         <v>422</v>
       </c>
@@ -16764,8 +18171,17 @@
       <c r="D422" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="423" spans="1:4">
+      <c r="E422" s="1" t="s">
+        <v>1976</v>
+      </c>
+      <c r="F422" s="2" t="s">
+        <v>2013</v>
+      </c>
+      <c r="G422" s="2" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="423" spans="1:11" ht="60">
       <c r="A423" s="1">
         <v>423</v>
       </c>
@@ -16778,8 +18194,14 @@
       <c r="D423" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="424" spans="1:4">
+      <c r="E423" s="1" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F423" s="2" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="424" spans="1:11" ht="330">
       <c r="A424" s="1">
         <v>424</v>
       </c>
@@ -16792,8 +18214,17 @@
       <c r="D424" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="425" spans="1:4">
+      <c r="E424" s="1" t="s">
+        <v>1978</v>
+      </c>
+      <c r="F424" s="2" t="s">
+        <v>2015</v>
+      </c>
+      <c r="G424" s="2" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="425" spans="1:11" ht="45">
       <c r="A425" s="1">
         <v>425</v>
       </c>
@@ -16806,8 +18237,14 @@
       <c r="D425" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="426" spans="1:4">
+      <c r="E425" s="1" t="s">
+        <v>1979</v>
+      </c>
+      <c r="F425" s="2" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="426" spans="1:11" ht="45">
       <c r="A426" s="1">
         <v>426</v>
       </c>
@@ -16820,8 +18257,17 @@
       <c r="D426" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="427" spans="1:4">
+      <c r="E426" s="1" t="s">
+        <v>1980</v>
+      </c>
+      <c r="F426" s="2" t="s">
+        <v>2017</v>
+      </c>
+      <c r="G426" s="2" t="s">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="427" spans="1:11" ht="30">
       <c r="A427" s="1">
         <v>427</v>
       </c>
@@ -16834,8 +18280,14 @@
       <c r="D427" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="428" spans="1:4">
+      <c r="E427" s="1" t="s">
+        <v>1981</v>
+      </c>
+      <c r="F427" s="2" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="428" spans="1:11" ht="45">
       <c r="A428" s="1">
         <v>428</v>
       </c>
@@ -16848,8 +18300,14 @@
       <c r="D428" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="429" spans="1:4">
+      <c r="E428" s="1" t="s">
+        <v>1982</v>
+      </c>
+      <c r="F428" s="2" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="429" spans="1:11" ht="30">
       <c r="A429" s="1">
         <v>429</v>
       </c>
@@ -16862,8 +18320,14 @@
       <c r="D429" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="430" spans="1:4">
+      <c r="E429" s="1" t="s">
+        <v>1983</v>
+      </c>
+      <c r="F429" s="2" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="430" spans="1:11" ht="45">
       <c r="A430" s="1">
         <v>430</v>
       </c>
@@ -16876,8 +18340,17 @@
       <c r="D430" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="431" spans="1:4">
+      <c r="E430" s="1" t="s">
+        <v>1984</v>
+      </c>
+      <c r="F430" s="2" t="s">
+        <v>2021</v>
+      </c>
+      <c r="G430" s="2" t="s">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="431" spans="1:11" ht="45">
       <c r="A431" s="1">
         <v>431</v>
       </c>
@@ -16890,8 +18363,17 @@
       <c r="D431" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="432" spans="1:4">
+      <c r="E431" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="F431" s="2" t="s">
+        <v>2022</v>
+      </c>
+      <c r="G431" s="2" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="432" spans="1:11" ht="210">
       <c r="A432" s="1">
         <v>432</v>
       </c>
@@ -16904,8 +18386,17 @@
       <c r="D432" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="433" spans="1:4">
+      <c r="E432" s="1" t="s">
+        <v>1986</v>
+      </c>
+      <c r="F432" s="2" t="s">
+        <v>1877</v>
+      </c>
+      <c r="G432" s="2" t="s">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="433" spans="1:11" ht="105">
       <c r="A433" s="1">
         <v>433</v>
       </c>
@@ -16918,8 +18409,17 @@
       <c r="D433" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="434" spans="1:4">
+      <c r="E433" s="1" t="s">
+        <v>1987</v>
+      </c>
+      <c r="F433" s="2" t="s">
+        <v>2023</v>
+      </c>
+      <c r="G433" s="2" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="434" spans="1:11" ht="120">
       <c r="A434" s="1">
         <v>434</v>
       </c>
@@ -16932,8 +18432,23 @@
       <c r="D434" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="435" spans="1:4">
+      <c r="E434" s="1" t="s">
+        <v>1988</v>
+      </c>
+      <c r="F434" s="2" t="s">
+        <v>2024</v>
+      </c>
+      <c r="G434" s="2" t="s">
+        <v>2043</v>
+      </c>
+      <c r="I434" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K434" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="435" spans="1:11" ht="165">
       <c r="A435" s="1">
         <v>435</v>
       </c>
@@ -16946,8 +18461,20 @@
       <c r="D435" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="436" spans="1:4">
+      <c r="E435" s="1" t="s">
+        <v>1989</v>
+      </c>
+      <c r="F435" s="2" t="s">
+        <v>2025</v>
+      </c>
+      <c r="G435" s="2" t="s">
+        <v>2040</v>
+      </c>
+      <c r="I435" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="436" spans="1:11" ht="75">
       <c r="A436" s="1">
         <v>436</v>
       </c>
@@ -16960,8 +18487,17 @@
       <c r="D436" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="437" spans="1:4">
+      <c r="E436" s="1" t="s">
+        <v>1990</v>
+      </c>
+      <c r="F436" s="2" t="s">
+        <v>2026</v>
+      </c>
+      <c r="G436" s="2" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="437" spans="1:11" ht="45">
       <c r="A437" s="1">
         <v>437</v>
       </c>
@@ -16974,8 +18510,17 @@
       <c r="D437" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="438" spans="1:4">
+      <c r="E437" s="1" t="s">
+        <v>1991</v>
+      </c>
+      <c r="F437" s="2" t="s">
+        <v>2027</v>
+      </c>
+      <c r="G437" s="2" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="438" spans="1:11" ht="75">
       <c r="A438" s="1">
         <v>438</v>
       </c>
@@ -16988,8 +18533,23 @@
       <c r="D438" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="439" spans="1:4">
+      <c r="E438" s="1" t="s">
+        <v>1992</v>
+      </c>
+      <c r="F438" s="2" t="s">
+        <v>2028</v>
+      </c>
+      <c r="G438" s="2" t="s">
+        <v>2049</v>
+      </c>
+      <c r="H438" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K438" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="439" spans="1:11" ht="75">
       <c r="A439" s="1">
         <v>439</v>
       </c>
@@ -17002,8 +18562,20 @@
       <c r="D439" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="440" spans="1:4">
+      <c r="E439" s="1" t="s">
+        <v>1993</v>
+      </c>
+      <c r="F439" s="2" t="s">
+        <v>2029</v>
+      </c>
+      <c r="G439" s="2" t="s">
+        <v>2050</v>
+      </c>
+      <c r="K439" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="440" spans="1:11" ht="150">
       <c r="A440" s="1">
         <v>440</v>
       </c>
@@ -17016,8 +18588,20 @@
       <c r="D440" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="441" spans="1:4">
+      <c r="E440" s="1" t="s">
+        <v>1994</v>
+      </c>
+      <c r="F440" s="2" t="s">
+        <v>2030</v>
+      </c>
+      <c r="G440" s="2" t="s">
+        <v>1829</v>
+      </c>
+      <c r="K440" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="441" spans="1:11" ht="75">
       <c r="A441" s="1">
         <v>441</v>
       </c>
@@ -17030,8 +18614,23 @@
       <c r="D441" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="442" spans="1:4">
+      <c r="E441" s="1" t="s">
+        <v>1995</v>
+      </c>
+      <c r="F441" s="2" t="s">
+        <v>2031</v>
+      </c>
+      <c r="G441" s="2" t="s">
+        <v>1886</v>
+      </c>
+      <c r="H441" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K441" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="442" spans="1:11" ht="60">
       <c r="A442" s="1">
         <v>442</v>
       </c>
@@ -17044,8 +18643,23 @@
       <c r="D442" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="443" spans="1:4">
+      <c r="E442" s="1" t="s">
+        <v>1996</v>
+      </c>
+      <c r="F442" s="2" t="s">
+        <v>2032</v>
+      </c>
+      <c r="G442" s="2" t="s">
+        <v>2051</v>
+      </c>
+      <c r="H442" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K442" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="443" spans="1:11" ht="60">
       <c r="A443" s="1">
         <v>443</v>
       </c>
@@ -17058,8 +18672,23 @@
       <c r="D443" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="444" spans="1:4">
+      <c r="E443" s="1" t="s">
+        <v>1997</v>
+      </c>
+      <c r="F443" s="2" t="s">
+        <v>2033</v>
+      </c>
+      <c r="G443" s="2" t="s">
+        <v>2052</v>
+      </c>
+      <c r="H443" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K443" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="444" spans="1:11" ht="225">
       <c r="A444" s="1">
         <v>444</v>
       </c>
@@ -17072,8 +18701,23 @@
       <c r="D444" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="445" spans="1:4">
+      <c r="E444" s="1" t="s">
+        <v>1998</v>
+      </c>
+      <c r="F444" s="2" t="s">
+        <v>2034</v>
+      </c>
+      <c r="G444" s="2" t="s">
+        <v>2006</v>
+      </c>
+      <c r="H444" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K444" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="445" spans="1:11" ht="60">
       <c r="A445" s="1">
         <v>445</v>
       </c>
@@ -17086,8 +18730,17 @@
       <c r="D445" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="446" spans="1:4">
+      <c r="E445" s="1" t="s">
+        <v>1999</v>
+      </c>
+      <c r="F445" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="G445" s="2" t="s">
+        <v>2051</v>
+      </c>
+    </row>
+    <row r="446" spans="1:11" ht="60">
       <c r="A446" s="1">
         <v>446</v>
       </c>
@@ -17100,8 +18753,20 @@
       <c r="D446" s="1" t="s">
         <v>1379</v>
       </c>
-    </row>
-    <row r="447" spans="1:4">
+      <c r="E446" s="1" t="s">
+        <v>2000</v>
+      </c>
+      <c r="F446" s="2" t="s">
+        <v>2036</v>
+      </c>
+      <c r="G446" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="I446" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="447" spans="1:11" ht="45">
       <c r="A447" s="1">
         <v>447</v>
       </c>
@@ -17113,11 +18778,23 @@
       </c>
       <c r="D447" s="1" t="s">
         <v>1379</v>
+      </c>
+      <c r="E447" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="F447" s="2" t="s">
+        <v>2037</v>
+      </c>
+      <c r="G447" s="2" t="s">
+        <v>2054</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0078D7 C1 - Interne</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -17129,23 +18806,23 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D51" activeCellId="1" sqref="B2 D51"/>
+      <selection pane="bottomRight" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" style="1" customWidth="1"/>
-    <col min="5" max="5" width="44.1328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="106.1328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="86.73046875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.73046875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1328125" style="1"/>
+    <col min="5" max="5" width="44.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="106.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="86.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
@@ -17888,7 +19565,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="28.5">
+    <row r="35" spans="1:8" ht="30">
       <c r="A35">
         <v>1034</v>
       </c>
@@ -17908,7 +19585,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="28.5">
+    <row r="36" spans="1:8" ht="30">
       <c r="A36">
         <v>1035</v>
       </c>
@@ -17928,7 +19605,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75">
+    <row r="37" spans="1:8" ht="30">
       <c r="A37">
         <v>1036</v>
       </c>
@@ -17974,7 +19651,7 @@
         <v>1709</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="28.5">
+    <row r="39" spans="1:8" ht="30">
       <c r="A39">
         <v>1038</v>
       </c>
@@ -18274,6 +19951,9 @@
       <c r="C52" s="15" t="s">
         <v>1379</v>
       </c>
+      <c r="D52" s="1" t="s">
+        <v>2038</v>
+      </c>
       <c r="G52" s="11" t="s">
         <v>1763</v>
       </c>
@@ -18290,6 +19970,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0078D7 C1 - Interne</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -18301,20 +19984,20 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C2" activeCellId="1" sqref="B2 C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" customWidth="1"/>
-    <col min="4" max="4" width="49.73046875" customWidth="1"/>
-    <col min="5" max="5" width="51.265625" customWidth="1"/>
-    <col min="6" max="6" width="19.265625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
@@ -18951,7 +20634,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0078D7 C1 - Interne</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -18965,11 +20648,11 @@
       <selection pane="bottomLeft" activeCellId="1" sqref="B2 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.3984375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="1"/>
+    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1">
@@ -19031,6 +20714,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0078D7 C1 - Interne</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -19046,10 +20732,10 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="11.53125" style="16"/>
+    <col min="2" max="2" width="11.5703125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -19075,7 +20761,13 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;KffffffStrona &amp;P_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K0078D7 C1 - Interne</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{ee0428da-ac0f-4a84-a429-a80e20cb35de}" enabled="1" method="Standard" siteId="{80c03608-5f64-40bb-9c70-9394abe6011c}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>